<commit_message>
desc, qty, unit price restructured df
</commit_message>
<xml_diff>
--- a/pwd/final_output.xlsx
+++ b/pwd/final_output.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -3015,6 +3015,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -3065,19 +3066,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -3086,10 +3087,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -3245,7 +3246,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -3254,13 +3255,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -3270,7 +3271,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -3279,7 +3280,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -3288,7 +3289,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -3298,12 +3299,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -3334,7 +3335,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -3353,7 +3354,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -3368,7 +3369,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BE134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -11654,6 +11657,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some more test and utility function.
</commit_message>
<xml_diff>
--- a/pwd/final_output.xlsx
+++ b/pwd/final_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2789" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2789" uniqueCount="951">
   <si>
     <t>dc_state</t>
   </si>
@@ -1902,6 +1902,9 @@
     <t>Mumbai Location – 5 Qty. Birla Aurora Tower, Level 17 &amp; 18,  Dr. Annie Besant Road, Worli, Mumbai 400030   Chennai Location :10 Qty. 5th Floor, Door no. 94, TVH Beliciaa towers, MRC Nagar, Chennai,  Tamil Nadu 600028</t>
   </si>
   <si>
+    <t xml:space="preserve">bangalore </t>
+  </si>
+  <si>
     <t xml:space="preserve"> -                 </t>
   </si>
   <si>
@@ -1996,6 +1999,9 @@
   </si>
   <si>
     <t>same state</t>
+  </si>
+  <si>
+    <t>sez</t>
   </si>
   <si>
     <t>interstate</t>
@@ -3488,19 +3494,19 @@
         <v>1</v>
       </c>
       <c r="Q2" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S2" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="T2" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U2" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
     <row r="3" spans="1:60">
@@ -3544,7 +3550,7 @@
         <v>459</v>
       </c>
       <c r="N3" t="s">
-        <v>531</v>
+        <v>617</v>
       </c>
       <c r="O3" t="s">
         <v>548</v>
@@ -3553,19 +3559,19 @@
         <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R3" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="S3" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="T3" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U3" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
     </row>
     <row r="4" spans="1:60">
@@ -3618,28 +3624,28 @@
         <v>2</v>
       </c>
       <c r="Q4" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R4" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S4" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="T4" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="U4" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="V4" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="W4" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="X4" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
     </row>
     <row r="5" spans="1:60">
@@ -3695,16 +3701,16 @@
         <v>530</v>
       </c>
       <c r="R5" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S5" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="T5" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="U5" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="6" spans="1:60">
@@ -3757,19 +3763,19 @@
         <v>1</v>
       </c>
       <c r="Q6" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R6" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S6" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="T6" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U6" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
     <row r="7" spans="1:60">
@@ -3822,19 +3828,19 @@
         <v>1</v>
       </c>
       <c r="Q7" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R7" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S7" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="T7" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U7" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="8" spans="1:60">
@@ -3887,19 +3893,19 @@
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S8" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="T8" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="U8" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
     </row>
     <row r="9" spans="1:60">
@@ -3952,19 +3958,19 @@
         <v>1</v>
       </c>
       <c r="Q9" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R9" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S9" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="T9" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U9" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
     </row>
     <row r="10" spans="1:60">
@@ -4017,73 +4023,73 @@
         <v>7</v>
       </c>
       <c r="Q10" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R10" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S10" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="T10" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="U10" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="V10" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="W10" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="X10" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="Y10" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="Z10" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="AA10" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="AB10" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="AC10" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="AD10" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="AE10" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="AF10" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="AG10" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="AH10" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="AI10" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="AJ10" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="AK10" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="AL10" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="AM10" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
     </row>
     <row r="11" spans="1:60">
@@ -4136,28 +4142,28 @@
         <v>2</v>
       </c>
       <c r="Q11" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R11" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S11" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="T11" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="U11" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="V11" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="W11" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="X11" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
     </row>
     <row r="12" spans="1:60">
@@ -4210,19 +4216,19 @@
         <v>1</v>
       </c>
       <c r="Q12" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R12" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S12" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="T12" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="U12" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
     <row r="13" spans="1:60">
@@ -4269,25 +4275,25 @@
         <v>530</v>
       </c>
       <c r="O13" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="P13">
         <v>1</v>
       </c>
       <c r="Q13" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R13" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S13" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="T13" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U13" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
     </row>
     <row r="14" spans="1:60">
@@ -4334,49 +4340,49 @@
         <v>530</v>
       </c>
       <c r="O14" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="P14">
         <v>7</v>
       </c>
       <c r="Q14" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R14" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S14" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="T14" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="U14" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="V14" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="AZ14" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="BA14" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="BC14" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="BD14" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="BF14" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="BG14" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="BH14" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
     </row>
     <row r="15" spans="1:60">
@@ -4423,49 +4429,49 @@
         <v>530</v>
       </c>
       <c r="O15" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="P15">
         <v>7</v>
       </c>
       <c r="Q15" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R15" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S15" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="T15" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="U15" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="V15" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="AZ15" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="BA15" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="BC15" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="BD15" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="BF15" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="BG15" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="BH15" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
     </row>
     <row r="16" spans="1:60">
@@ -4521,16 +4527,16 @@
         <v>530</v>
       </c>
       <c r="R16" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S16" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="T16" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="U16" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -4586,16 +4592,16 @@
         <v>530</v>
       </c>
       <c r="R17" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S17" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="T17" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="U17" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -4648,19 +4654,19 @@
         <v>1</v>
       </c>
       <c r="Q18" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R18" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S18" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="T18" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U18" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -4716,16 +4722,16 @@
         <v>530</v>
       </c>
       <c r="R19" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S19" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="T19" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="U19" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -4781,34 +4787,34 @@
         <v>530</v>
       </c>
       <c r="R20" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S20" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="T20" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="U20" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="V20" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="W20" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="X20" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="Y20" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="Z20" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="AA20" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -4861,19 +4867,19 @@
         <v>1</v>
       </c>
       <c r="Q21" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R21" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S21" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="T21" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U21" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -4926,19 +4932,19 @@
         <v>1</v>
       </c>
       <c r="Q22" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R22" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S22" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="T22" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U22" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -4991,19 +4997,19 @@
         <v>1</v>
       </c>
       <c r="Q23" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R23" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S23" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="T23" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="U23" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
     <row r="24" spans="1:27">
@@ -5056,19 +5062,19 @@
         <v>1</v>
       </c>
       <c r="Q24" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R24" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S24" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="T24" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="U24" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -5121,19 +5127,19 @@
         <v>1</v>
       </c>
       <c r="Q25" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R25" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S25" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="T25" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U25" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -5189,16 +5195,16 @@
         <v>530</v>
       </c>
       <c r="R26" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S26" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="T26" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="U26" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="27" spans="1:27">
@@ -5254,16 +5260,16 @@
         <v>530</v>
       </c>
       <c r="R27" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S27" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="T27" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="U27" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -5316,19 +5322,19 @@
         <v>1</v>
       </c>
       <c r="Q28" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R28" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S28" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="T28" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U28" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
     <row r="29" spans="1:27">
@@ -5375,43 +5381,43 @@
         <v>530</v>
       </c>
       <c r="O29" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="P29">
         <v>3</v>
       </c>
       <c r="Q29" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R29" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S29" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="T29" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="U29" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="V29" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="W29" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X29" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="Y29" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="Z29" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="AA29" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
     </row>
     <row r="30" spans="1:27">
@@ -5464,19 +5470,19 @@
         <v>1</v>
       </c>
       <c r="Q30" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R30" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S30" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="T30" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U30" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
     </row>
     <row r="31" spans="1:27">
@@ -5529,19 +5535,19 @@
         <v>1</v>
       </c>
       <c r="Q31" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R31" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S31" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="T31" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U31" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -5594,28 +5600,28 @@
         <v>2</v>
       </c>
       <c r="Q32" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R32" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S32" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="T32" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U32" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="V32" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="W32" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X32" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
     </row>
     <row r="33" spans="1:39">
@@ -5668,19 +5674,19 @@
         <v>1</v>
       </c>
       <c r="Q33" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R33" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S33" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="T33" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U33" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
     </row>
     <row r="34" spans="1:39">
@@ -5733,73 +5739,73 @@
         <v>7</v>
       </c>
       <c r="Q34" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R34" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S34" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="T34" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="U34" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="V34" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="W34" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="X34" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="Y34" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="Z34" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="AA34" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="AB34" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="AC34" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="AD34" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="AE34" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="AF34" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="AG34" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="AH34" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="AI34" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="AJ34" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="AK34" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="AL34" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="AM34" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
     </row>
     <row r="35" spans="1:39">
@@ -5843,22 +5849,22 @@
         <v>530</v>
       </c>
       <c r="O35" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="P35">
         <v>1</v>
       </c>
       <c r="R35" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S35" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="T35" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U35" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="36" spans="1:39">
@@ -5914,16 +5920,16 @@
         <v>530</v>
       </c>
       <c r="R36" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S36" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="T36" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="U36" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="37" spans="1:39">
@@ -5979,16 +5985,16 @@
         <v>530</v>
       </c>
       <c r="R37" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S37" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="T37" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="U37" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
     </row>
     <row r="38" spans="1:39">
@@ -6035,43 +6041,43 @@
         <v>530</v>
       </c>
       <c r="O38" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="P38">
         <v>3</v>
       </c>
       <c r="Q38" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R38" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S38" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="T38" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="U38" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="V38" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="W38" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="X38" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="Y38" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="Z38" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="AA38" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
     </row>
     <row r="39" spans="1:39">
@@ -6124,19 +6130,19 @@
         <v>1</v>
       </c>
       <c r="Q39" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R39" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S39" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="T39" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U39" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
     </row>
     <row r="40" spans="1:39">
@@ -6189,19 +6195,19 @@
         <v>1</v>
       </c>
       <c r="Q40" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R40" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S40" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="T40" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U40" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
     <row r="41" spans="1:39">
@@ -6254,19 +6260,19 @@
         <v>1</v>
       </c>
       <c r="Q41" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R41" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S41" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="T41" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U41" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="42" spans="1:39">
@@ -6319,19 +6325,19 @@
         <v>1</v>
       </c>
       <c r="Q42" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R42" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S42" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="T42" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U42" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
     </row>
     <row r="43" spans="1:39">
@@ -6384,19 +6390,19 @@
         <v>1</v>
       </c>
       <c r="Q43" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R43" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S43" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="T43" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U43" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="44" spans="1:39">
@@ -6449,19 +6455,19 @@
         <v>1</v>
       </c>
       <c r="Q44" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R44" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S44" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="T44" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U44" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="45" spans="1:39">
@@ -6514,19 +6520,19 @@
         <v>1</v>
       </c>
       <c r="Q45" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R45" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S45" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="T45" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U45" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="46" spans="1:39">
@@ -6579,19 +6585,19 @@
         <v>1</v>
       </c>
       <c r="Q46" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R46" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S46" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="T46" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U46" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="47" spans="1:39">
@@ -6644,46 +6650,46 @@
         <v>4</v>
       </c>
       <c r="Q47" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R47" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S47" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="T47" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="U47" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="V47" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="W47" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="X47" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="Y47" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="Z47" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="AA47" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="AB47" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="AC47" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="AD47" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
     </row>
     <row r="48" spans="1:39">
@@ -6736,19 +6742,19 @@
         <v>1</v>
       </c>
       <c r="Q48" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R48" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S48" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="T48" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U48" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
     </row>
     <row r="49" spans="1:39">
@@ -6801,19 +6807,19 @@
         <v>1</v>
       </c>
       <c r="Q49" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R49" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S49" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="T49" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U49" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
     </row>
     <row r="50" spans="1:39">
@@ -6866,19 +6872,19 @@
         <v>1</v>
       </c>
       <c r="Q50" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R50" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S50" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="T50" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U50" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
     </row>
     <row r="51" spans="1:39">
@@ -6925,79 +6931,79 @@
         <v>530</v>
       </c>
       <c r="O51" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="P51">
         <v>7</v>
       </c>
       <c r="Q51" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R51" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S51" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="T51" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="U51" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="V51" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="W51" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="X51" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="Y51" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="Z51" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="AA51" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="AB51" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="AC51" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="AD51" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="AE51" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="AF51" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="AG51" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="AH51" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="AI51" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="AJ51" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="AK51" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="AL51" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="AM51" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
     </row>
     <row r="52" spans="1:39">
@@ -7050,19 +7056,19 @@
         <v>1</v>
       </c>
       <c r="Q52" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R52" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S52" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="T52" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U52" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="53" spans="1:39">
@@ -7115,64 +7121,64 @@
         <v>6</v>
       </c>
       <c r="Q53" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R53" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S53" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="T53" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="U53" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="V53" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="W53" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="X53" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="Y53" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="Z53" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="AA53" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="AB53" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="AC53" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="AD53" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="AE53" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="AF53" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="AG53" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="AH53" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="AI53" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="AJ53" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
     </row>
     <row r="54" spans="1:39">
@@ -7225,19 +7231,19 @@
         <v>1</v>
       </c>
       <c r="Q54" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R54" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S54" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="T54" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U54" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
     </row>
     <row r="55" spans="1:39">
@@ -7290,19 +7296,19 @@
         <v>1</v>
       </c>
       <c r="Q55" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R55" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S55" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="T55" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U55" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
     </row>
     <row r="56" spans="1:39">
@@ -7352,19 +7358,19 @@
         <v>1</v>
       </c>
       <c r="Q56" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R56" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S56" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="T56" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="U56" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="57" spans="1:39">
@@ -7417,19 +7423,19 @@
         <v>1</v>
       </c>
       <c r="Q57" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R57" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S57" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="T57" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U57" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
     </row>
     <row r="58" spans="1:39">
@@ -7482,19 +7488,19 @@
         <v>1</v>
       </c>
       <c r="Q58" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R58" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S58" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="T58" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="U58" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="59" spans="1:39">
@@ -7547,19 +7553,19 @@
         <v>1</v>
       </c>
       <c r="Q59" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R59" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S59" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="T59" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="U59" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="60" spans="1:39">
@@ -7603,22 +7609,22 @@
         <v>530</v>
       </c>
       <c r="O60" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="P60">
         <v>1</v>
       </c>
       <c r="R60" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S60" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="T60" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U60" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="61" spans="1:39">
@@ -7671,19 +7677,19 @@
         <v>1</v>
       </c>
       <c r="Q61" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R61" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S61" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="T61" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="U61" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="62" spans="1:39">
@@ -7736,19 +7742,19 @@
         <v>1</v>
       </c>
       <c r="Q62" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R62" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S62" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="T62" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="U62" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
     </row>
     <row r="63" spans="1:39">
@@ -7798,19 +7804,19 @@
         <v>1</v>
       </c>
       <c r="Q63" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R63" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S63" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="T63" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="U63" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
     </row>
     <row r="64" spans="1:39">
@@ -7860,19 +7866,19 @@
         <v>1</v>
       </c>
       <c r="Q64" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R64" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S64" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="T64" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="U64" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="65" spans="1:51">
@@ -7925,19 +7931,19 @@
         <v>1</v>
       </c>
       <c r="Q65" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R65" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S65" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="T65" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="U65" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="66" spans="1:51">
@@ -7981,22 +7987,22 @@
         <v>530</v>
       </c>
       <c r="O66" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="P66">
         <v>1</v>
       </c>
       <c r="R66" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S66" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="T66" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U66" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="67" spans="1:51">
@@ -8049,19 +8055,19 @@
         <v>1</v>
       </c>
       <c r="Q67" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R67" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S67" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="T67" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="U67" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
     </row>
     <row r="68" spans="1:51">
@@ -8114,19 +8120,19 @@
         <v>1</v>
       </c>
       <c r="Q68" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R68" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S68" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="T68" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U68" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="69" spans="1:51">
@@ -8179,19 +8185,19 @@
         <v>1</v>
       </c>
       <c r="Q69" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R69" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S69" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="T69" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U69" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
     </row>
     <row r="70" spans="1:51">
@@ -8244,19 +8250,19 @@
         <v>1</v>
       </c>
       <c r="Q70" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R70" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S70" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="T70" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="U70" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="71" spans="1:51">
@@ -8309,28 +8315,28 @@
         <v>2</v>
       </c>
       <c r="Q71" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R71" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S71" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="T71" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U71" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="V71" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="W71" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X71" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
     </row>
     <row r="72" spans="1:51">
@@ -8374,22 +8380,22 @@
         <v>530</v>
       </c>
       <c r="O72" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="P72">
         <v>1</v>
       </c>
       <c r="R72" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S72" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="T72" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U72" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
     </row>
     <row r="73" spans="1:51">
@@ -8436,115 +8442,115 @@
         <v>531</v>
       </c>
       <c r="O73" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="P73">
         <v>11</v>
       </c>
       <c r="Q73" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="R73" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S73" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="T73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U73" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="V73" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="W73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X73" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="Y73" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="Z73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AA73" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="AB73" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="AC73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AD73" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="AE73" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="AF73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AG73" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="AH73" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="AI73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AJ73" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="AK73" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="AL73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AM73" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="AN73" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="AO73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AP73" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="AQ73" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="AR73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AS73" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="AT73" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="AU73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AV73" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="AW73" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="AX73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AY73" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
     </row>
     <row r="74" spans="1:51">
@@ -8591,25 +8597,25 @@
         <v>533</v>
       </c>
       <c r="O74" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="P74">
         <v>1</v>
       </c>
       <c r="Q74" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="R74" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S74" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="T74" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U74" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
     </row>
     <row r="75" spans="1:51">
@@ -8656,25 +8662,25 @@
         <v>535</v>
       </c>
       <c r="O75" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="P75">
         <v>1</v>
       </c>
       <c r="Q75" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="R75" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S75" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="T75" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U75" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
     </row>
     <row r="76" spans="1:51">
@@ -8721,61 +8727,61 @@
         <v>530</v>
       </c>
       <c r="O76" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="P76">
         <v>5</v>
       </c>
       <c r="Q76" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R76" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S76" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="T76" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U76" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="V76" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="W76" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X76" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="Y76" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="Z76" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AA76" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="AB76" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="AC76" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AD76" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="AE76" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="AF76" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="AG76" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
     </row>
     <row r="77" spans="1:51">
@@ -8822,34 +8828,34 @@
         <v>530</v>
       </c>
       <c r="O77" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="P77">
         <v>2</v>
       </c>
       <c r="Q77" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R77" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S77" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="T77" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U77" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="V77" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="W77" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X77" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
     </row>
     <row r="78" spans="1:51">
@@ -8896,25 +8902,25 @@
         <v>530</v>
       </c>
       <c r="O78" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="P78">
         <v>1</v>
       </c>
       <c r="Q78" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R78" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S78" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="T78" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U78" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
     </row>
     <row r="79" spans="1:51">
@@ -8961,25 +8967,25 @@
         <v>530</v>
       </c>
       <c r="O79" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="P79">
         <v>1</v>
       </c>
       <c r="Q79" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R79" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S79" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="T79" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="U79" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
     </row>
     <row r="80" spans="1:51">
@@ -9026,25 +9032,25 @@
         <v>530</v>
       </c>
       <c r="O80" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="P80">
         <v>1</v>
       </c>
       <c r="Q80" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R80" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S80" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="T80" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U80" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
     </row>
     <row r="81" spans="1:57">
@@ -9097,19 +9103,19 @@
         <v>1</v>
       </c>
       <c r="Q81" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R81" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S81" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="T81" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U81" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="82" spans="1:57">
@@ -9162,19 +9168,19 @@
         <v>1</v>
       </c>
       <c r="Q82" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R82" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S82" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="T82" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U82" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
     <row r="83" spans="1:57">
@@ -9227,19 +9233,19 @@
         <v>1</v>
       </c>
       <c r="Q83" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R83" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S83" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="T83" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U83" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
     <row r="84" spans="1:57">
@@ -9283,22 +9289,22 @@
         <v>530</v>
       </c>
       <c r="O84" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="P84">
         <v>1</v>
       </c>
       <c r="R84" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S84" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="T84" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="U84" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
     </row>
     <row r="85" spans="1:57">
@@ -9345,61 +9351,61 @@
         <v>530</v>
       </c>
       <c r="O85" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="P85">
         <v>6</v>
       </c>
       <c r="Q85" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="R85" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S85" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="T85" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="U85" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="V85" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="W85" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="X85" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="AN85" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="AO85" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="AP85" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="AZ85" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="BA85" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="BB85" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="BC85" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="BD85" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="BE85" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
     </row>
     <row r="86" spans="1:57">
@@ -9446,25 +9452,25 @@
         <v>530</v>
       </c>
       <c r="O86" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="P86">
         <v>1</v>
       </c>
       <c r="Q86" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R86" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S86" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="T86" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="U86" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
     </row>
     <row r="87" spans="1:57">
@@ -9511,34 +9517,34 @@
         <v>530</v>
       </c>
       <c r="O87" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="P87">
         <v>2</v>
       </c>
       <c r="Q87" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R87" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S87" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="T87" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U87" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="V87" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="W87" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X87" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
     </row>
     <row r="88" spans="1:57">
@@ -9585,25 +9591,25 @@
         <v>530</v>
       </c>
       <c r="O88" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="P88">
         <v>1</v>
       </c>
       <c r="Q88" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R88" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S88" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="T88" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="U88" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
     </row>
     <row r="89" spans="1:57">
@@ -9650,34 +9656,34 @@
         <v>536</v>
       </c>
       <c r="O89" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="P89">
         <v>2</v>
       </c>
       <c r="Q89" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R89" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S89" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="T89" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="U89" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="V89" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="W89" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X89" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
     </row>
     <row r="90" spans="1:57">
@@ -9724,34 +9730,34 @@
         <v>530</v>
       </c>
       <c r="O90" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="P90">
         <v>2</v>
       </c>
       <c r="Q90" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R90" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S90" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="T90" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="U90" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="V90" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="W90" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="X90" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
     </row>
     <row r="91" spans="1:57">
@@ -9798,25 +9804,25 @@
         <v>530</v>
       </c>
       <c r="O91" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="P91">
         <v>1</v>
       </c>
       <c r="Q91" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R91" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S91" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="T91" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U91" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
     </row>
     <row r="92" spans="1:57">
@@ -9863,25 +9869,25 @@
         <v>530</v>
       </c>
       <c r="O92" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="P92">
         <v>1</v>
       </c>
       <c r="Q92" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R92" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S92" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="T92" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="U92" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
     </row>
     <row r="93" spans="1:57">
@@ -9928,25 +9934,25 @@
         <v>531</v>
       </c>
       <c r="O93" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="P93">
         <v>1</v>
       </c>
       <c r="Q93" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R93" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S93" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="T93" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="U93" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
     </row>
     <row r="94" spans="1:57">
@@ -9993,25 +9999,25 @@
         <v>531</v>
       </c>
       <c r="O94" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="P94">
         <v>1</v>
       </c>
       <c r="Q94" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R94" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S94" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="T94" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="U94" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
     </row>
     <row r="95" spans="1:57">
@@ -10055,25 +10061,25 @@
         <v>530</v>
       </c>
       <c r="O95" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="P95">
         <v>1</v>
       </c>
       <c r="Q95" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R95" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S95" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="T95" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="U95" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
     </row>
     <row r="96" spans="1:57">
@@ -10120,25 +10126,25 @@
         <v>531</v>
       </c>
       <c r="O96" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="P96">
         <v>1</v>
       </c>
       <c r="Q96" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R96" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S96" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="T96" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="U96" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
     </row>
     <row r="97" spans="1:24">
@@ -10185,25 +10191,25 @@
         <v>531</v>
       </c>
       <c r="O97" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="P97">
         <v>1</v>
       </c>
       <c r="Q97" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="R97" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S97" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="T97" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="U97" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
     </row>
     <row r="98" spans="1:24">
@@ -10244,34 +10250,34 @@
         <v>530</v>
       </c>
       <c r="O98" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="P98">
         <v>2</v>
       </c>
       <c r="Q98" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R98" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S98" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="T98" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="U98" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="V98" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="W98" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="X98" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
     </row>
     <row r="99" spans="1:24">
@@ -10315,19 +10321,19 @@
         <v>1</v>
       </c>
       <c r="Q99" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R99" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S99" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="T99" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U99" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
     </row>
     <row r="100" spans="1:24">
@@ -10374,25 +10380,25 @@
         <v>530</v>
       </c>
       <c r="O100" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="P100">
         <v>1</v>
       </c>
       <c r="Q100" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R100" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S100" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="T100" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U100" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
     </row>
     <row r="101" spans="1:24">
@@ -10439,25 +10445,25 @@
         <v>530</v>
       </c>
       <c r="O101" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="P101">
         <v>1</v>
       </c>
       <c r="Q101" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R101" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S101" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="T101" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U101" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
     </row>
     <row r="102" spans="1:24">
@@ -10504,25 +10510,25 @@
         <v>530</v>
       </c>
       <c r="O102" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="P102">
         <v>1</v>
       </c>
       <c r="Q102" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R102" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S102" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="T102" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U102" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
     </row>
     <row r="103" spans="1:24">
@@ -10563,16 +10569,16 @@
         <v>530</v>
       </c>
       <c r="O103" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="P103">
         <v>1</v>
       </c>
       <c r="Q103" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R103" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="104" spans="1:24">
@@ -10613,16 +10619,16 @@
         <v>530</v>
       </c>
       <c r="O104" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="P104">
         <v>1</v>
       </c>
       <c r="Q104" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R104" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="105" spans="1:24">
@@ -10669,25 +10675,25 @@
         <v>530</v>
       </c>
       <c r="O105" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="P105">
         <v>1</v>
       </c>
       <c r="Q105" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R105" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S105" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="T105" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="U105" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="106" spans="1:24">
@@ -10734,25 +10740,25 @@
         <v>530</v>
       </c>
       <c r="O106" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="P106">
         <v>1</v>
       </c>
       <c r="Q106" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R106" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S106" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="T106" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="U106" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
     </row>
     <row r="107" spans="1:24">
@@ -10799,25 +10805,25 @@
         <v>530</v>
       </c>
       <c r="O107" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="P107">
         <v>1</v>
       </c>
       <c r="Q107" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R107" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S107" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="T107" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="U107" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
     </row>
     <row r="108" spans="1:24">
@@ -10858,34 +10864,34 @@
         <v>530</v>
       </c>
       <c r="O108" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="P108">
         <v>2</v>
       </c>
       <c r="Q108" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R108" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S108" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="T108" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U108" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="V108" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="W108" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X108" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="109" spans="1:24">
@@ -10926,34 +10932,34 @@
         <v>530</v>
       </c>
       <c r="O109" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="P109">
         <v>2</v>
       </c>
       <c r="Q109" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R109" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S109" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="T109" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U109" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="V109" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="W109" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X109" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="110" spans="1:24">
@@ -11000,16 +11006,16 @@
         <v>530</v>
       </c>
       <c r="O110" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="P110">
         <v>1</v>
       </c>
       <c r="Q110" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R110" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="111" spans="1:24">
@@ -11056,16 +11062,16 @@
         <v>530</v>
       </c>
       <c r="O111" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="P111">
         <v>1</v>
       </c>
       <c r="Q111" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R111" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="112" spans="1:24">
@@ -11112,25 +11118,25 @@
         <v>530</v>
       </c>
       <c r="O112" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="P112">
         <v>1</v>
       </c>
       <c r="Q112" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R112" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S112" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="T112" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U112" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
     </row>
     <row r="113" spans="1:36">
@@ -11177,25 +11183,25 @@
         <v>530</v>
       </c>
       <c r="O113" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="P113">
         <v>1</v>
       </c>
       <c r="Q113" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R113" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S113" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="T113" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U113" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
     </row>
     <row r="114" spans="1:36">
@@ -11242,25 +11248,25 @@
         <v>530</v>
       </c>
       <c r="O114" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="P114">
         <v>1</v>
       </c>
       <c r="Q114" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R114" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S114" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="T114" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="U114" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="115" spans="1:36">
@@ -11307,25 +11313,25 @@
         <v>530</v>
       </c>
       <c r="O115" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="P115">
         <v>1</v>
       </c>
       <c r="Q115" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R115" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S115" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="T115" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U115" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
     </row>
     <row r="116" spans="1:36">
@@ -11378,10 +11384,10 @@
         <v>1</v>
       </c>
       <c r="Q116" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R116" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="117" spans="1:36">
@@ -11428,25 +11434,25 @@
         <v>530</v>
       </c>
       <c r="O117" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="P117">
         <v>1</v>
       </c>
       <c r="Q117" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R117" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S117" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="T117" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U117" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
     </row>
     <row r="118" spans="1:36">
@@ -11493,34 +11499,34 @@
         <v>530</v>
       </c>
       <c r="O118" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="P118">
         <v>2</v>
       </c>
       <c r="Q118" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R118" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S118" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="T118" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U118" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="V118" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="W118" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="X118" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
     </row>
     <row r="119" spans="1:36">
@@ -11561,22 +11567,22 @@
         <v>530</v>
       </c>
       <c r="O119" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="P119">
         <v>1</v>
       </c>
       <c r="R119" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S119" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="T119" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U119" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
     </row>
     <row r="120" spans="1:36">
@@ -11623,52 +11629,52 @@
         <v>539</v>
       </c>
       <c r="O120" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="P120">
         <v>4</v>
       </c>
       <c r="Q120" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R120" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S120" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="T120" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U120" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="V120" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="W120" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="X120" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="Y120" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="Z120" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AA120" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="AB120" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="AC120" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AD120" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
     <row r="121" spans="1:36">
@@ -11715,52 +11721,52 @@
         <v>539</v>
       </c>
       <c r="O121" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="P121">
         <v>4</v>
       </c>
       <c r="Q121" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R121" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S121" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="T121" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U121" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="V121" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="W121" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="X121" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="Y121" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="Z121" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AA121" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="AB121" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="AC121" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AD121" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
     <row r="122" spans="1:36">
@@ -11807,52 +11813,52 @@
         <v>541</v>
       </c>
       <c r="O122" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="P122">
         <v>4</v>
       </c>
       <c r="Q122" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R122" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S122" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="T122" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U122" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="V122" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="W122" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="X122" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="Y122" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="Z122" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AA122" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="AB122" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="AC122" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AD122" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
     <row r="123" spans="1:36">
@@ -11899,70 +11905,70 @@
         <v>542</v>
       </c>
       <c r="O123" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="P123">
         <v>6</v>
       </c>
       <c r="Q123" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R123" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S123" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="T123" t="s">
+        <v>743</v>
+      </c>
+      <c r="U123" t="s">
+        <v>844</v>
+      </c>
+      <c r="V123" t="s">
+        <v>866</v>
+      </c>
+      <c r="W123" t="s">
+        <v>743</v>
+      </c>
+      <c r="X123" t="s">
+        <v>885</v>
+      </c>
+      <c r="Y123" t="s">
+        <v>894</v>
+      </c>
+      <c r="Z123" t="s">
+        <v>738</v>
+      </c>
+      <c r="AA123" t="s">
+        <v>904</v>
+      </c>
+      <c r="AB123" t="s">
+        <v>912</v>
+      </c>
+      <c r="AC123" t="s">
+        <v>738</v>
+      </c>
+      <c r="AD123" t="s">
+        <v>917</v>
+      </c>
+      <c r="AE123" t="s">
+        <v>922</v>
+      </c>
+      <c r="AF123" t="s">
         <v>741</v>
       </c>
-      <c r="U123" t="s">
-        <v>842</v>
-      </c>
-      <c r="V123" t="s">
-        <v>864</v>
-      </c>
-      <c r="W123" t="s">
+      <c r="AG123" t="s">
+        <v>929</v>
+      </c>
+      <c r="AH123" t="s">
+        <v>933</v>
+      </c>
+      <c r="AI123" t="s">
         <v>741</v>
       </c>
-      <c r="X123" t="s">
-        <v>883</v>
-      </c>
-      <c r="Y123" t="s">
-        <v>892</v>
-      </c>
-      <c r="Z123" t="s">
-        <v>736</v>
-      </c>
-      <c r="AA123" t="s">
-        <v>902</v>
-      </c>
-      <c r="AB123" t="s">
-        <v>910</v>
-      </c>
-      <c r="AC123" t="s">
-        <v>736</v>
-      </c>
-      <c r="AD123" t="s">
-        <v>915</v>
-      </c>
-      <c r="AE123" t="s">
-        <v>920</v>
-      </c>
-      <c r="AF123" t="s">
-        <v>739</v>
-      </c>
-      <c r="AG123" t="s">
-        <v>927</v>
-      </c>
-      <c r="AH123" t="s">
-        <v>931</v>
-      </c>
-      <c r="AI123" t="s">
-        <v>739</v>
-      </c>
       <c r="AJ123" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
     </row>
     <row r="124" spans="1:36">
@@ -12009,25 +12015,25 @@
         <v>543</v>
       </c>
       <c r="O124" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="P124">
         <v>1</v>
       </c>
       <c r="Q124" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R124" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S124" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="T124" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="U124" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="125" spans="1:36">
@@ -12074,25 +12080,25 @@
         <v>543</v>
       </c>
       <c r="O125" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="P125">
         <v>1</v>
       </c>
       <c r="Q125" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R125" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S125" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="T125" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="U125" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="126" spans="1:36">
@@ -12139,25 +12145,25 @@
         <v>543</v>
       </c>
       <c r="O126" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="P126">
         <v>1</v>
       </c>
       <c r="Q126" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R126" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S126" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="T126" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="U126" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="127" spans="1:36">
@@ -12204,25 +12210,25 @@
         <v>543</v>
       </c>
       <c r="O127" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="P127">
         <v>1</v>
       </c>
       <c r="Q127" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R127" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S127" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="T127" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="U127" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="128" spans="1:36">
@@ -12269,25 +12275,25 @@
         <v>543</v>
       </c>
       <c r="O128" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="P128">
         <v>1</v>
       </c>
       <c r="Q128" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R128" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S128" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="T128" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="U128" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="129" spans="1:24">
@@ -12337,16 +12343,16 @@
         <v>1</v>
       </c>
       <c r="Q129" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R129" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S129" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="U129" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
     </row>
     <row r="130" spans="1:24">
@@ -12393,25 +12399,25 @@
         <v>530</v>
       </c>
       <c r="O130" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="P130">
         <v>1</v>
       </c>
       <c r="Q130" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R130" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="S130" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="T130" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U130" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
     </row>
     <row r="131" spans="1:24">
@@ -12458,34 +12464,34 @@
         <v>544</v>
       </c>
       <c r="O131" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="P131">
         <v>2</v>
       </c>
       <c r="Q131" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="R131" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S131" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="T131" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="U131" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="V131" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="W131" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="X131" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
     </row>
     <row r="132" spans="1:24">
@@ -12532,34 +12538,34 @@
         <v>544</v>
       </c>
       <c r="O132" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="P132">
         <v>2</v>
       </c>
       <c r="Q132" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="R132" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S132" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="T132" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="U132" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="V132" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="W132" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="X132" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
     </row>
     <row r="133" spans="1:24">
@@ -12606,25 +12612,25 @@
         <v>545</v>
       </c>
       <c r="O133" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="P133">
         <v>1</v>
       </c>
       <c r="Q133" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R133" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S133" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="T133" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U133" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
     </row>
     <row r="134" spans="1:24">
@@ -12677,19 +12683,19 @@
         <v>1</v>
       </c>
       <c r="Q134" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R134" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="S134" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="T134" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U134" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed unnecessary data from freight
</commit_message>
<xml_diff>
--- a/pwd/final_output.xlsx
+++ b/pwd/final_output.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rishabh\Desktop\rpa projects\rpae_project\19thDecember\pwd\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3893" uniqueCount="1006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3845" uniqueCount="997">
   <si>
     <t>dc_state</t>
   </si>
@@ -1481,7 +1486,7 @@
 Off Andheri Kurla Road Andheri - East</t>
   </si>
   <si>
-    <t xml:space="preserve">310,  Hammersmith ,  Narayan Pathare Marg,     Off Sitladevi Temple Road
+    <t>310,  Hammersmith ,  Narayan Pathare Marg,     Off Sitladevi Temple Road
   Mahim (West),  Mumbai - 400 016.  Psychical material deliver on this address  (mail attached ) Protolab Electrotechnologies Pvt. Ltd. EL 93,  Electronic Zone,  Block A  Road No.16
  MIDC,  TTC Industrial Area,  Mahape,  Navi Mumbai - 400 709  </t>
   </si>
@@ -1646,7 +1651,7 @@
 Thane-West,  Thane-400604</t>
   </si>
   <si>
-    <t xml:space="preserve">310,  Hammersmith ,  Narayan Pathare Marg
+    <t>310,  Hammersmith ,  Narayan Pathare Marg
     Off Sitladevi Temple Road,   Mahim (West),  Mumbai - 400 016.  Psychical material deliver on this address  (mail attached ) Jaspal / CMPCS Compound,  Near Libra Kata
   Kalamboli,  Panvel,  Navi,  Mumbai- 410218.  Mr. Anil Jadhav  / 022-27420112    </t>
   </si>
@@ -2304,34 +2309,7 @@
     <t>5554</t>
   </si>
   <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>00.00</t>
-  </si>
-  <si>
-    <t>Nil</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Inclusive</t>
-  </si>
-  <si>
-    <t>INCL.</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>697380.00</t>
   </si>
   <si>
     <t>ThinkPad Battery 68+ (6 cell) For T440s, X240, T450s, X250, X260, L450, L460 Laptop Part No: 0C52862 HSN Code: 85078000</t>
@@ -3225,8 +3203,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3289,6 +3267,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3335,7 +3321,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3367,9 +3353,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3401,6 +3388,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3576,14 +3564,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:58">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3756,7 +3746,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:58">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3833,16 +3823,16 @@
         <v>699</v>
       </c>
       <c r="Z2" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="AA2" t="s">
         <v>639</v>
       </c>
       <c r="AB2" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
     </row>
-    <row r="3" spans="1:58">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3916,16 +3906,16 @@
         <v>687</v>
       </c>
       <c r="Z3" t="s">
-        <v>711</v>
+        <v>702</v>
       </c>
       <c r="AA3" t="s">
         <v>639</v>
       </c>
       <c r="AB3" t="s">
-        <v>828</v>
+        <v>819</v>
       </c>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3999,25 +3989,25 @@
         <v>687</v>
       </c>
       <c r="Z4" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
       <c r="AA4" t="s">
         <v>646</v>
       </c>
       <c r="AB4" t="s">
-        <v>829</v>
+        <v>820</v>
       </c>
       <c r="AC4" t="s">
-        <v>906</v>
+        <v>897</v>
       </c>
       <c r="AD4" t="s">
         <v>646</v>
       </c>
       <c r="AE4" t="s">
-        <v>925</v>
+        <v>916</v>
       </c>
     </row>
-    <row r="5" spans="1:58">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4090,20 +4080,17 @@
       <c r="X5" t="s">
         <v>688</v>
       </c>
-      <c r="Y5" t="s">
-        <v>700</v>
-      </c>
       <c r="Z5" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="AA5" t="s">
         <v>642</v>
       </c>
       <c r="AB5" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
     </row>
-    <row r="6" spans="1:58">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4177,16 +4164,16 @@
         <v>687</v>
       </c>
       <c r="Z6" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
       <c r="AA6" t="s">
         <v>639</v>
       </c>
       <c r="AB6" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4260,16 +4247,16 @@
         <v>687</v>
       </c>
       <c r="Z7" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
       <c r="AA7" t="s">
         <v>639</v>
       </c>
       <c r="AB7" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
-    <row r="8" spans="1:58">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4343,16 +4330,16 @@
         <v>687</v>
       </c>
       <c r="Z8" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="AA8" t="s">
         <v>640</v>
       </c>
       <c r="AB8" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
     </row>
-    <row r="9" spans="1:58">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4414,16 +4401,16 @@
         <v>687</v>
       </c>
       <c r="Z9" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="AA9" t="s">
         <v>639</v>
       </c>
       <c r="AB9" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
     </row>
-    <row r="10" spans="1:58">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4497,16 +4484,16 @@
         <v>687</v>
       </c>
       <c r="Z10" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="AA10" t="s">
         <v>639</v>
       </c>
       <c r="AB10" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
     </row>
-    <row r="11" spans="1:58">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4580,70 +4567,70 @@
         <v>687</v>
       </c>
       <c r="Z11" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="AA11" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
       <c r="AB11" t="s">
-        <v>834</v>
+        <v>825</v>
       </c>
       <c r="AC11" t="s">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="AD11" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
       <c r="AE11" t="s">
-        <v>926</v>
+        <v>917</v>
       </c>
       <c r="AF11" t="s">
+        <v>934</v>
+      </c>
+      <c r="AG11" t="s">
         <v>943</v>
       </c>
-      <c r="AG11" t="s">
-        <v>952</v>
-      </c>
       <c r="AH11" t="s">
+        <v>944</v>
+      </c>
+      <c r="AI11" t="s">
         <v>953</v>
       </c>
-      <c r="AI11" t="s">
-        <v>962</v>
-      </c>
       <c r="AJ11" t="s">
-        <v>952</v>
+        <v>943</v>
       </c>
       <c r="AK11" t="s">
-        <v>926</v>
+        <v>917</v>
       </c>
       <c r="AL11" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="AM11" t="s">
-        <v>980</v>
+        <v>971</v>
       </c>
       <c r="AN11" t="s">
-        <v>981</v>
+        <v>972</v>
       </c>
       <c r="AO11" t="s">
-        <v>963</v>
+        <v>954</v>
       </c>
       <c r="AP11" t="s">
-        <v>980</v>
+        <v>971</v>
       </c>
       <c r="AQ11" t="s">
-        <v>991</v>
+        <v>982</v>
       </c>
       <c r="AR11" t="s">
-        <v>994</v>
+        <v>985</v>
       </c>
       <c r="AS11" t="s">
-        <v>980</v>
+        <v>971</v>
       </c>
       <c r="AT11" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
     </row>
-    <row r="12" spans="1:58">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -4717,25 +4704,25 @@
         <v>687</v>
       </c>
       <c r="Z12" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
       <c r="AA12" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
       <c r="AB12" t="s">
-        <v>829</v>
+        <v>820</v>
       </c>
       <c r="AC12" t="s">
-        <v>906</v>
+        <v>897</v>
       </c>
       <c r="AD12" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
       <c r="AE12" t="s">
-        <v>925</v>
+        <v>916</v>
       </c>
     </row>
-    <row r="13" spans="1:58">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4809,16 +4796,16 @@
         <v>687</v>
       </c>
       <c r="Z13" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="AA13" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
       <c r="AB13" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
     </row>
-    <row r="14" spans="1:58">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4888,20 +4875,17 @@
       <c r="X14" t="s">
         <v>689</v>
       </c>
-      <c r="Y14" t="s">
-        <v>701</v>
-      </c>
       <c r="Z14" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
       <c r="AA14" t="s">
         <v>639</v>
       </c>
       <c r="AB14" t="s">
-        <v>836</v>
+        <v>827</v>
       </c>
     </row>
-    <row r="15" spans="1:58">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4975,22 +4959,22 @@
         <v>689</v>
       </c>
       <c r="Y15" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="Z15" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="AA15" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="AB15" t="s">
         <v>639</v>
       </c>
       <c r="AC15" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
     </row>
-    <row r="16" spans="1:58">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -5064,22 +5048,22 @@
         <v>689</v>
       </c>
       <c r="Y16" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="Z16" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="AA16" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="AB16" t="s">
         <v>639</v>
       </c>
       <c r="AC16" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
     </row>
-    <row r="17" spans="1:34">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -5152,20 +5136,17 @@
       <c r="X17" t="s">
         <v>688</v>
       </c>
-      <c r="Y17" t="s">
-        <v>703</v>
-      </c>
       <c r="Z17" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="AA17" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
       <c r="AB17" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
     </row>
-    <row r="18" spans="1:34">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -5238,20 +5219,17 @@
       <c r="X18" t="s">
         <v>688</v>
       </c>
-      <c r="Y18" t="s">
-        <v>703</v>
-      </c>
       <c r="Z18" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="AA18" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="AB18" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
     </row>
-    <row r="19" spans="1:34">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -5325,16 +5303,16 @@
         <v>687</v>
       </c>
       <c r="Z19" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="AA19" t="s">
         <v>639</v>
       </c>
       <c r="AB19" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
     </row>
-    <row r="20" spans="1:34">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -5407,20 +5385,17 @@
       <c r="X20" t="s">
         <v>688</v>
       </c>
-      <c r="Y20" t="s">
-        <v>703</v>
-      </c>
       <c r="Z20" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="AA20" t="s">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="AB20" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
     </row>
-    <row r="21" spans="1:34">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -5493,38 +5468,35 @@
       <c r="X21" t="s">
         <v>688</v>
       </c>
-      <c r="Y21" t="s">
-        <v>703</v>
-      </c>
       <c r="Z21" t="s">
-        <v>725</v>
+        <v>716</v>
       </c>
       <c r="AA21" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
       <c r="AB21" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
       <c r="AC21" t="s">
-        <v>725</v>
+        <v>716</v>
       </c>
       <c r="AD21" t="s">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="AE21" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
       <c r="AF21" t="s">
-        <v>725</v>
+        <v>716</v>
       </c>
       <c r="AG21" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="AH21" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="22" spans="1:34">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -5598,16 +5570,16 @@
         <v>687</v>
       </c>
       <c r="Z22" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="AA22" t="s">
         <v>639</v>
       </c>
       <c r="AB22" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
     </row>
-    <row r="23" spans="1:34">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -5681,16 +5653,16 @@
         <v>687</v>
       </c>
       <c r="Z23" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="AA23" t="s">
         <v>639</v>
       </c>
       <c r="AB23" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
     </row>
-    <row r="24" spans="1:34">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -5764,16 +5736,16 @@
         <v>687</v>
       </c>
       <c r="Z24" t="s">
-        <v>726</v>
+        <v>717</v>
       </c>
       <c r="AA24" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
       <c r="AB24" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
     </row>
-    <row r="25" spans="1:34">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -5847,16 +5819,16 @@
         <v>687</v>
       </c>
       <c r="Z25" t="s">
-        <v>727</v>
+        <v>718</v>
       </c>
       <c r="AA25" t="s">
         <v>640</v>
       </c>
       <c r="AB25" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
-    <row r="26" spans="1:34">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -5930,16 +5902,16 @@
         <v>687</v>
       </c>
       <c r="Z26" t="s">
-        <v>728</v>
+        <v>719</v>
       </c>
       <c r="AA26" t="s">
         <v>639</v>
       </c>
       <c r="AB26" t="s">
-        <v>841</v>
+        <v>832</v>
       </c>
     </row>
-    <row r="27" spans="1:34">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -6012,20 +5984,17 @@
       <c r="X27" t="s">
         <v>690</v>
       </c>
-      <c r="Y27" t="s">
-        <v>704</v>
-      </c>
       <c r="Z27" t="s">
-        <v>729</v>
+        <v>720</v>
       </c>
       <c r="AA27" t="s">
-        <v>808</v>
+        <v>799</v>
       </c>
       <c r="AB27" t="s">
-        <v>842</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="28" spans="1:34">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -6098,20 +6067,17 @@
       <c r="X28" t="s">
         <v>688</v>
       </c>
-      <c r="Y28" t="s">
-        <v>703</v>
-      </c>
       <c r="Z28" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="AA28" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="AB28" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
     </row>
-    <row r="29" spans="1:34">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -6184,20 +6150,17 @@
       <c r="X29" t="s">
         <v>688</v>
       </c>
-      <c r="Y29" t="s">
-        <v>703</v>
-      </c>
       <c r="Z29" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="AA29" t="s">
         <v>645</v>
       </c>
       <c r="AB29" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
     </row>
-    <row r="30" spans="1:34">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -6271,16 +6234,16 @@
         <v>687</v>
       </c>
       <c r="Z30" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="AA30" t="s">
         <v>639</v>
       </c>
       <c r="AB30" t="s">
-        <v>843</v>
+        <v>834</v>
       </c>
     </row>
-    <row r="31" spans="1:34">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -6353,38 +6316,35 @@
       <c r="X31" t="s">
         <v>689</v>
       </c>
-      <c r="Y31" t="s">
-        <v>704</v>
-      </c>
       <c r="Z31" t="s">
-        <v>730</v>
+        <v>721</v>
       </c>
       <c r="AA31" t="s">
         <v>640</v>
       </c>
       <c r="AB31" t="s">
-        <v>844</v>
+        <v>835</v>
       </c>
       <c r="AC31" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="AD31" t="s">
         <v>639</v>
       </c>
       <c r="AE31" t="s">
-        <v>927</v>
+        <v>918</v>
       </c>
       <c r="AF31" t="s">
-        <v>944</v>
+        <v>935</v>
       </c>
       <c r="AG31" t="s">
         <v>640</v>
       </c>
       <c r="AH31" t="s">
-        <v>954</v>
+        <v>945</v>
       </c>
     </row>
-    <row r="32" spans="1:34">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -6458,16 +6418,16 @@
         <v>687</v>
       </c>
       <c r="Z32" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
       <c r="AA32" t="s">
         <v>639</v>
       </c>
       <c r="AB32" t="s">
-        <v>845</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="33" spans="1:46">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -6541,16 +6501,16 @@
         <v>687</v>
       </c>
       <c r="Z33" t="s">
-        <v>727</v>
+        <v>718</v>
       </c>
       <c r="AA33" t="s">
         <v>639</v>
       </c>
       <c r="AB33" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
-    <row r="34" spans="1:46">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -6624,25 +6584,25 @@
         <v>687</v>
       </c>
       <c r="Z34" t="s">
-        <v>732</v>
+        <v>723</v>
       </c>
       <c r="AA34" t="s">
         <v>639</v>
       </c>
       <c r="AB34" t="s">
-        <v>846</v>
+        <v>837</v>
       </c>
       <c r="AC34" t="s">
-        <v>909</v>
+        <v>900</v>
       </c>
       <c r="AD34" t="s">
         <v>639</v>
       </c>
       <c r="AE34" t="s">
-        <v>928</v>
+        <v>919</v>
       </c>
     </row>
-    <row r="35" spans="1:46">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -6716,16 +6676,16 @@
         <v>687</v>
       </c>
       <c r="Z35" t="s">
-        <v>732</v>
+        <v>723</v>
       </c>
       <c r="AA35" t="s">
         <v>639</v>
       </c>
       <c r="AB35" t="s">
-        <v>846</v>
+        <v>837</v>
       </c>
     </row>
-    <row r="36" spans="1:46">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -6799,70 +6759,70 @@
         <v>687</v>
       </c>
       <c r="Z36" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="AA36" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="AB36" t="s">
-        <v>847</v>
+        <v>838</v>
       </c>
       <c r="AC36" t="s">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="AD36" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="AE36" t="s">
-        <v>929</v>
+        <v>920</v>
       </c>
       <c r="AF36" t="s">
-        <v>943</v>
+        <v>934</v>
       </c>
       <c r="AG36" t="s">
         <v>646</v>
       </c>
       <c r="AH36" t="s">
-        <v>955</v>
+        <v>946</v>
       </c>
       <c r="AI36" t="s">
-        <v>962</v>
+        <v>953</v>
       </c>
       <c r="AJ36" t="s">
         <v>646</v>
       </c>
       <c r="AK36" t="s">
-        <v>929</v>
+        <v>920</v>
       </c>
       <c r="AL36" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="AM36" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="AN36" t="s">
-        <v>982</v>
+        <v>973</v>
       </c>
       <c r="AO36" t="s">
-        <v>963</v>
+        <v>954</v>
       </c>
       <c r="AP36" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="AQ36" t="s">
-        <v>970</v>
+        <v>961</v>
       </c>
       <c r="AR36" t="s">
-        <v>994</v>
+        <v>985</v>
       </c>
       <c r="AS36" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="AT36" t="s">
-        <v>998</v>
+        <v>989</v>
       </c>
     </row>
-    <row r="37" spans="1:46">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -6936,16 +6896,16 @@
         <v>687</v>
       </c>
       <c r="Z37" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="AA37" t="s">
         <v>639</v>
       </c>
       <c r="AB37" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
-    <row r="38" spans="1:46">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -7018,20 +6978,17 @@
       <c r="X38" t="s">
         <v>688</v>
       </c>
-      <c r="Y38" t="s">
-        <v>703</v>
-      </c>
       <c r="Z38" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="AA38" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="AB38" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
     </row>
-    <row r="39" spans="1:46">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -7104,20 +7061,17 @@
       <c r="X39" t="s">
         <v>688</v>
       </c>
-      <c r="Y39" t="s">
-        <v>703</v>
-      </c>
       <c r="Z39" t="s">
-        <v>734</v>
+        <v>725</v>
       </c>
       <c r="AA39" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="AB39" t="s">
-        <v>848</v>
+        <v>839</v>
       </c>
     </row>
-    <row r="40" spans="1:46">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -7190,38 +7144,35 @@
       <c r="X40" t="s">
         <v>691</v>
       </c>
-      <c r="Y40" t="s">
-        <v>704</v>
-      </c>
       <c r="Z40" t="s">
-        <v>735</v>
+        <v>726</v>
       </c>
       <c r="AA40" t="s">
         <v>643</v>
       </c>
       <c r="AB40" t="s">
-        <v>849</v>
+        <v>840</v>
       </c>
       <c r="AC40" t="s">
-        <v>910</v>
+        <v>901</v>
       </c>
       <c r="AD40" t="s">
         <v>643</v>
       </c>
       <c r="AE40" t="s">
-        <v>930</v>
+        <v>921</v>
       </c>
       <c r="AF40" t="s">
-        <v>945</v>
+        <v>936</v>
       </c>
       <c r="AG40" t="s">
         <v>643</v>
       </c>
       <c r="AH40" t="s">
-        <v>956</v>
+        <v>947</v>
       </c>
     </row>
-    <row r="41" spans="1:46">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -7295,16 +7246,16 @@
         <v>687</v>
       </c>
       <c r="Z41" t="s">
-        <v>736</v>
+        <v>727</v>
       </c>
       <c r="AA41" t="s">
         <v>639</v>
       </c>
       <c r="AB41" t="s">
-        <v>850</v>
+        <v>841</v>
       </c>
     </row>
-    <row r="42" spans="1:46">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -7366,16 +7317,16 @@
         <v>687</v>
       </c>
       <c r="Z42" t="s">
-        <v>737</v>
+        <v>728</v>
       </c>
       <c r="AA42" t="s">
         <v>639</v>
       </c>
       <c r="AB42" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
     </row>
-    <row r="43" spans="1:46">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -7449,16 +7400,16 @@
         <v>687</v>
       </c>
       <c r="Z43" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="AA43" t="s">
         <v>639</v>
       </c>
       <c r="AB43" t="s">
-        <v>843</v>
+        <v>834</v>
       </c>
     </row>
-    <row r="44" spans="1:46">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -7532,16 +7483,16 @@
         <v>687</v>
       </c>
       <c r="Z44" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="AA44" t="s">
         <v>639</v>
       </c>
       <c r="AB44" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
     </row>
-    <row r="45" spans="1:46">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -7615,16 +7566,16 @@
         <v>687</v>
       </c>
       <c r="Z45" t="s">
-        <v>737</v>
+        <v>728</v>
       </c>
       <c r="AA45" t="s">
         <v>639</v>
       </c>
       <c r="AB45" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
     </row>
-    <row r="46" spans="1:46">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -7698,16 +7649,16 @@
         <v>687</v>
       </c>
       <c r="Z46" t="s">
-        <v>738</v>
+        <v>729</v>
       </c>
       <c r="AA46" t="s">
         <v>639</v>
       </c>
       <c r="AB46" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
     </row>
-    <row r="47" spans="1:46">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -7769,16 +7720,16 @@
         <v>687</v>
       </c>
       <c r="Z47" t="s">
-        <v>737</v>
+        <v>728</v>
       </c>
       <c r="AA47" t="s">
         <v>639</v>
       </c>
       <c r="AB47" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
     </row>
-    <row r="48" spans="1:46">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -7852,16 +7803,16 @@
         <v>687</v>
       </c>
       <c r="Z48" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="AA48" t="s">
         <v>639</v>
       </c>
       <c r="AB48" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
     </row>
-    <row r="49" spans="1:46">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -7935,16 +7886,16 @@
         <v>687</v>
       </c>
       <c r="Z49" t="s">
-        <v>727</v>
+        <v>718</v>
       </c>
       <c r="AA49" t="s">
         <v>639</v>
       </c>
       <c r="AB49" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
-    <row r="50" spans="1:46">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -8018,16 +7969,16 @@
         <v>687</v>
       </c>
       <c r="Z50" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="AA50" t="s">
         <v>639</v>
       </c>
       <c r="AB50" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
     </row>
-    <row r="51" spans="1:46">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -8100,47 +8051,44 @@
       <c r="X51" t="s">
         <v>687</v>
       </c>
-      <c r="Y51" t="s">
-        <v>705</v>
-      </c>
       <c r="Z51" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="AA51" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="AB51" t="s">
-        <v>852</v>
+        <v>843</v>
       </c>
       <c r="AC51" t="s">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="AD51" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="AE51" t="s">
-        <v>931</v>
+        <v>922</v>
       </c>
       <c r="AF51" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="AG51" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="AH51" t="s">
-        <v>957</v>
+        <v>948</v>
       </c>
       <c r="AI51" t="s">
-        <v>963</v>
+        <v>954</v>
       </c>
       <c r="AJ51" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AK51" t="s">
-        <v>970</v>
+        <v>961</v>
       </c>
     </row>
-    <row r="52" spans="1:46">
+    <row r="52" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -8214,16 +8162,16 @@
         <v>687</v>
       </c>
       <c r="Z52" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="AA52" t="s">
         <v>639</v>
       </c>
       <c r="AB52" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
     </row>
-    <row r="53" spans="1:46">
+    <row r="53" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -8297,16 +8245,16 @@
         <v>687</v>
       </c>
       <c r="Z53" t="s">
-        <v>739</v>
+        <v>730</v>
       </c>
       <c r="AA53" t="s">
         <v>639</v>
       </c>
       <c r="AB53" t="s">
-        <v>853</v>
+        <v>844</v>
       </c>
     </row>
-    <row r="54" spans="1:46">
+    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -8380,16 +8328,16 @@
         <v>687</v>
       </c>
       <c r="Z54" t="s">
-        <v>740</v>
+        <v>731</v>
       </c>
       <c r="AA54" t="s">
         <v>639</v>
       </c>
       <c r="AB54" t="s">
-        <v>854</v>
+        <v>845</v>
       </c>
     </row>
-    <row r="55" spans="1:46">
+    <row r="55" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -8459,74 +8407,71 @@
       <c r="X55" t="s">
         <v>689</v>
       </c>
-      <c r="Y55" t="s">
-        <v>701</v>
-      </c>
       <c r="Z55" t="s">
-        <v>741</v>
+        <v>732</v>
       </c>
       <c r="AA55" t="s">
         <v>646</v>
       </c>
       <c r="AB55" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
       <c r="AC55" t="s">
-        <v>911</v>
+        <v>902</v>
       </c>
       <c r="AD55" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AE55" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
       <c r="AF55" t="s">
-        <v>946</v>
+        <v>937</v>
       </c>
       <c r="AG55" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AH55" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
       <c r="AI55" t="s">
-        <v>964</v>
+        <v>955</v>
       </c>
       <c r="AJ55" t="s">
         <v>646</v>
       </c>
       <c r="AK55" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
       <c r="AL55" t="s">
-        <v>975</v>
+        <v>966</v>
       </c>
       <c r="AM55" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AN55" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
       <c r="AO55" t="s">
-        <v>987</v>
+        <v>978</v>
       </c>
       <c r="AP55" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AQ55" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
       <c r="AR55" t="s">
-        <v>995</v>
+        <v>986</v>
       </c>
       <c r="AS55" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AT55" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
     </row>
-    <row r="56" spans="1:46">
+    <row r="56" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -8600,16 +8545,16 @@
         <v>687</v>
       </c>
       <c r="Z56" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="AA56" t="s">
         <v>639</v>
       </c>
       <c r="AB56" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
-    <row r="57" spans="1:46">
+    <row r="57" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -8682,65 +8627,62 @@
       <c r="X57" t="s">
         <v>687</v>
       </c>
-      <c r="Y57" t="s">
-        <v>705</v>
-      </c>
       <c r="Z57" t="s">
-        <v>742</v>
+        <v>733</v>
       </c>
       <c r="AA57" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AB57" t="s">
-        <v>856</v>
+        <v>847</v>
       </c>
       <c r="AC57" t="s">
-        <v>912</v>
+        <v>903</v>
       </c>
       <c r="AD57" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AE57" t="s">
-        <v>932</v>
+        <v>923</v>
       </c>
       <c r="AF57" t="s">
-        <v>947</v>
+        <v>938</v>
       </c>
       <c r="AG57" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AH57" t="s">
-        <v>958</v>
+        <v>949</v>
       </c>
       <c r="AI57" t="s">
-        <v>965</v>
+        <v>956</v>
       </c>
       <c r="AJ57" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AK57" t="s">
-        <v>971</v>
+        <v>962</v>
       </c>
       <c r="AL57" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="AM57" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AN57" t="s">
-        <v>983</v>
+        <v>974</v>
       </c>
       <c r="AO57" t="s">
-        <v>988</v>
+        <v>979</v>
       </c>
       <c r="AP57" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AQ57" t="s">
-        <v>925</v>
+        <v>916</v>
       </c>
     </row>
-    <row r="58" spans="1:46">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -8814,16 +8756,16 @@
         <v>687</v>
       </c>
       <c r="Z58" t="s">
-        <v>743</v>
+        <v>734</v>
       </c>
       <c r="AA58" t="s">
         <v>639</v>
       </c>
       <c r="AB58" t="s">
-        <v>857</v>
+        <v>848</v>
       </c>
     </row>
-    <row r="59" spans="1:46">
+    <row r="59" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -8897,16 +8839,16 @@
         <v>687</v>
       </c>
       <c r="Z59" t="s">
-        <v>744</v>
+        <v>735</v>
       </c>
       <c r="AA59" t="s">
         <v>639</v>
       </c>
       <c r="AB59" t="s">
-        <v>858</v>
+        <v>849</v>
       </c>
     </row>
-    <row r="60" spans="1:46">
+    <row r="60" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -8979,20 +8921,17 @@
       <c r="X60" t="s">
         <v>687</v>
       </c>
-      <c r="Y60" t="s">
-        <v>705</v>
-      </c>
       <c r="Z60" t="s">
-        <v>745</v>
+        <v>736</v>
       </c>
       <c r="AA60" t="s">
         <v>641</v>
       </c>
       <c r="AB60" t="s">
-        <v>859</v>
+        <v>850</v>
       </c>
     </row>
-    <row r="61" spans="1:46">
+    <row r="61" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -9066,16 +9005,16 @@
         <v>687</v>
       </c>
       <c r="Z61" t="s">
-        <v>746</v>
+        <v>737</v>
       </c>
       <c r="AA61" t="s">
         <v>639</v>
       </c>
       <c r="AB61" t="s">
-        <v>860</v>
+        <v>851</v>
       </c>
     </row>
-    <row r="62" spans="1:46">
+    <row r="62" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -9149,16 +9088,16 @@
         <v>687</v>
       </c>
       <c r="Z62" t="s">
-        <v>745</v>
+        <v>736</v>
       </c>
       <c r="AA62" t="s">
         <v>643</v>
       </c>
       <c r="AB62" t="s">
-        <v>859</v>
+        <v>850</v>
       </c>
     </row>
-    <row r="63" spans="1:46">
+    <row r="63" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -9232,16 +9171,16 @@
         <v>687</v>
       </c>
       <c r="Z63" t="s">
-        <v>745</v>
+        <v>736</v>
       </c>
       <c r="AA63" t="s">
         <v>644</v>
       </c>
       <c r="AB63" t="s">
-        <v>859</v>
+        <v>850</v>
       </c>
     </row>
-    <row r="64" spans="1:46">
+    <row r="64" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -9315,16 +9254,16 @@
         <v>687</v>
       </c>
       <c r="Z64" t="s">
-        <v>747</v>
+        <v>738</v>
       </c>
       <c r="AA64" t="s">
         <v>639</v>
       </c>
       <c r="AB64" t="s">
-        <v>861</v>
+        <v>852</v>
       </c>
     </row>
-    <row r="65" spans="1:58">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -9398,16 +9337,16 @@
         <v>687</v>
       </c>
       <c r="Z65" t="s">
-        <v>745</v>
+        <v>736</v>
       </c>
       <c r="AA65" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="AB65" t="s">
-        <v>859</v>
+        <v>850</v>
       </c>
     </row>
-    <row r="66" spans="1:58">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -9481,16 +9420,16 @@
         <v>687</v>
       </c>
       <c r="Z66" t="s">
-        <v>748</v>
+        <v>739</v>
       </c>
       <c r="AA66" t="s">
         <v>640</v>
       </c>
       <c r="AB66" t="s">
-        <v>862</v>
+        <v>853</v>
       </c>
     </row>
-    <row r="67" spans="1:58">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -9563,20 +9502,17 @@
       <c r="X67" t="s">
         <v>687</v>
       </c>
-      <c r="Y67" t="s">
-        <v>705</v>
-      </c>
       <c r="Z67" t="s">
-        <v>748</v>
+        <v>739</v>
       </c>
       <c r="AA67" t="s">
         <v>640</v>
       </c>
       <c r="AB67" t="s">
-        <v>862</v>
+        <v>853</v>
       </c>
     </row>
-    <row r="68" spans="1:58">
+    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -9649,20 +9585,17 @@
       <c r="X68" t="s">
         <v>687</v>
       </c>
-      <c r="Y68" t="s">
-        <v>705</v>
-      </c>
       <c r="Z68" t="s">
-        <v>745</v>
+        <v>736</v>
       </c>
       <c r="AA68" t="s">
         <v>641</v>
       </c>
       <c r="AB68" t="s">
-        <v>859</v>
+        <v>850</v>
       </c>
     </row>
-    <row r="69" spans="1:58">
+    <row r="69" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -9736,16 +9669,16 @@
         <v>687</v>
       </c>
       <c r="Z69" t="s">
-        <v>745</v>
+        <v>736</v>
       </c>
       <c r="AA69" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
       <c r="AB69" t="s">
-        <v>859</v>
+        <v>850</v>
       </c>
     </row>
-    <row r="70" spans="1:58">
+    <row r="70" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -9819,16 +9752,16 @@
         <v>687</v>
       </c>
       <c r="Z70" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="AA70" t="s">
         <v>639</v>
       </c>
       <c r="AB70" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
-    <row r="71" spans="1:58">
+    <row r="71" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -9902,16 +9835,16 @@
         <v>687</v>
       </c>
       <c r="Z71" t="s">
-        <v>749</v>
+        <v>740</v>
       </c>
       <c r="AA71" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="AB71" t="s">
-        <v>863</v>
+        <v>854</v>
       </c>
     </row>
-    <row r="72" spans="1:58">
+    <row r="72" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -9985,16 +9918,16 @@
         <v>687</v>
       </c>
       <c r="Z72" t="s">
-        <v>750</v>
+        <v>741</v>
       </c>
       <c r="AA72" t="s">
         <v>639</v>
       </c>
       <c r="AB72" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
-    <row r="73" spans="1:58">
+    <row r="73" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -10068,16 +10001,16 @@
         <v>687</v>
       </c>
       <c r="Z73" t="s">
-        <v>751</v>
+        <v>742</v>
       </c>
       <c r="AA73" t="s">
         <v>639</v>
       </c>
       <c r="AB73" t="s">
-        <v>864</v>
+        <v>855</v>
       </c>
     </row>
-    <row r="74" spans="1:58">
+    <row r="74" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -10151,16 +10084,16 @@
         <v>687</v>
       </c>
       <c r="Z74" t="s">
-        <v>750</v>
+        <v>741</v>
       </c>
       <c r="AA74" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AB74" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
-    <row r="75" spans="1:58">
+    <row r="75" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -10234,25 +10167,25 @@
         <v>687</v>
       </c>
       <c r="Z75" t="s">
-        <v>752</v>
+        <v>743</v>
       </c>
       <c r="AA75" t="s">
         <v>639</v>
       </c>
       <c r="AB75" t="s">
-        <v>865</v>
+        <v>856</v>
       </c>
       <c r="AC75" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="AD75" t="s">
         <v>639</v>
       </c>
       <c r="AE75" t="s">
-        <v>933</v>
+        <v>924</v>
       </c>
     </row>
-    <row r="76" spans="1:58">
+    <row r="76" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -10326,16 +10259,16 @@
         <v>687</v>
       </c>
       <c r="Z76" t="s">
-        <v>753</v>
+        <v>744</v>
       </c>
       <c r="AA76" t="s">
         <v>639</v>
       </c>
       <c r="AB76" t="s">
-        <v>866</v>
+        <v>857</v>
       </c>
     </row>
-    <row r="77" spans="1:58">
+    <row r="77" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -10405,110 +10338,107 @@
       <c r="X77" t="s">
         <v>689</v>
       </c>
-      <c r="Y77" t="s">
-        <v>701</v>
-      </c>
       <c r="Z77" t="s">
-        <v>754</v>
+        <v>745</v>
       </c>
       <c r="AA77" t="s">
         <v>639</v>
       </c>
       <c r="AB77" t="s">
-        <v>867</v>
+        <v>858</v>
       </c>
       <c r="AC77" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="AD77" t="s">
         <v>639</v>
       </c>
       <c r="AE77" t="s">
-        <v>934</v>
+        <v>925</v>
       </c>
       <c r="AF77" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="AG77" t="s">
         <v>639</v>
       </c>
       <c r="AH77" t="s">
-        <v>959</v>
+        <v>950</v>
       </c>
       <c r="AI77" t="s">
-        <v>966</v>
+        <v>957</v>
       </c>
       <c r="AJ77" t="s">
         <v>639</v>
       </c>
       <c r="AK77" t="s">
-        <v>972</v>
+        <v>963</v>
       </c>
       <c r="AL77" t="s">
-        <v>977</v>
+        <v>968</v>
       </c>
       <c r="AM77" t="s">
         <v>639</v>
       </c>
       <c r="AN77" t="s">
-        <v>984</v>
+        <v>975</v>
       </c>
       <c r="AO77" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="AP77" t="s">
         <v>639</v>
       </c>
       <c r="AQ77" t="s">
+        <v>983</v>
+      </c>
+      <c r="AR77" t="s">
+        <v>987</v>
+      </c>
+      <c r="AS77" t="s">
+        <v>639</v>
+      </c>
+      <c r="AT77" t="s">
+        <v>990</v>
+      </c>
+      <c r="AU77" t="s">
+        <v>991</v>
+      </c>
+      <c r="AV77" t="s">
+        <v>639</v>
+      </c>
+      <c r="AW77" t="s">
+        <v>860</v>
+      </c>
+      <c r="AX77" t="s">
         <v>992</v>
       </c>
-      <c r="AR77" t="s">
+      <c r="AY77" t="s">
+        <v>639</v>
+      </c>
+      <c r="AZ77" t="s">
+        <v>876</v>
+      </c>
+      <c r="BA77" t="s">
+        <v>993</v>
+      </c>
+      <c r="BB77" t="s">
+        <v>639</v>
+      </c>
+      <c r="BC77" t="s">
+        <v>994</v>
+      </c>
+      <c r="BD77" t="s">
+        <v>995</v>
+      </c>
+      <c r="BE77" t="s">
+        <v>639</v>
+      </c>
+      <c r="BF77" t="s">
         <v>996</v>
       </c>
-      <c r="AS77" t="s">
-        <v>639</v>
-      </c>
-      <c r="AT77" t="s">
-        <v>999</v>
-      </c>
-      <c r="AU77" t="s">
-        <v>1000</v>
-      </c>
-      <c r="AV77" t="s">
-        <v>639</v>
-      </c>
-      <c r="AW77" t="s">
-        <v>869</v>
-      </c>
-      <c r="AX77" t="s">
-        <v>1001</v>
-      </c>
-      <c r="AY77" t="s">
-        <v>639</v>
-      </c>
-      <c r="AZ77" t="s">
-        <v>885</v>
-      </c>
-      <c r="BA77" t="s">
-        <v>1002</v>
-      </c>
-      <c r="BB77" t="s">
-        <v>639</v>
-      </c>
-      <c r="BC77" t="s">
-        <v>1003</v>
-      </c>
-      <c r="BD77" t="s">
-        <v>1004</v>
-      </c>
-      <c r="BE77" t="s">
-        <v>639</v>
-      </c>
-      <c r="BF77" t="s">
-        <v>1005</v>
-      </c>
     </row>
-    <row r="78" spans="1:58">
+    <row r="78" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -10578,20 +10508,17 @@
       <c r="X78" t="s">
         <v>689</v>
       </c>
-      <c r="Y78" t="s">
-        <v>701</v>
-      </c>
       <c r="Z78" t="s">
-        <v>755</v>
+        <v>746</v>
       </c>
       <c r="AA78" t="s">
         <v>639</v>
       </c>
       <c r="AB78" t="s">
-        <v>868</v>
+        <v>859</v>
       </c>
     </row>
-    <row r="79" spans="1:58">
+    <row r="79" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -10661,20 +10588,17 @@
       <c r="X79" t="s">
         <v>689</v>
       </c>
-      <c r="Y79" t="s">
-        <v>701</v>
-      </c>
       <c r="Z79" t="s">
-        <v>756</v>
+        <v>747</v>
       </c>
       <c r="AA79" t="s">
         <v>639</v>
       </c>
       <c r="AB79" t="s">
-        <v>869</v>
+        <v>860</v>
       </c>
     </row>
-    <row r="80" spans="1:58">
+    <row r="80" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -10744,56 +10668,53 @@
       <c r="X80" t="s">
         <v>689</v>
       </c>
-      <c r="Y80" t="s">
-        <v>701</v>
-      </c>
       <c r="Z80" t="s">
-        <v>757</v>
+        <v>748</v>
       </c>
       <c r="AA80" t="s">
         <v>639</v>
       </c>
       <c r="AB80" t="s">
-        <v>870</v>
+        <v>861</v>
       </c>
       <c r="AC80" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
       <c r="AD80" t="s">
         <v>639</v>
       </c>
       <c r="AE80" t="s">
-        <v>935</v>
+        <v>926</v>
       </c>
       <c r="AF80" t="s">
-        <v>949</v>
+        <v>940</v>
       </c>
       <c r="AG80" t="s">
         <v>639</v>
       </c>
       <c r="AH80" t="s">
-        <v>960</v>
+        <v>951</v>
       </c>
       <c r="AI80" t="s">
-        <v>967</v>
+        <v>958</v>
       </c>
       <c r="AJ80" t="s">
         <v>639</v>
       </c>
       <c r="AK80" t="s">
-        <v>973</v>
+        <v>964</v>
       </c>
       <c r="AL80" t="s">
-        <v>978</v>
+        <v>969</v>
       </c>
       <c r="AM80" t="s">
         <v>640</v>
       </c>
       <c r="AN80" t="s">
-        <v>985</v>
+        <v>976</v>
       </c>
     </row>
-    <row r="81" spans="1:49">
+    <row r="81" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -10863,29 +10784,26 @@
       <c r="X81" t="s">
         <v>689</v>
       </c>
-      <c r="Y81" t="s">
-        <v>701</v>
-      </c>
       <c r="Z81" t="s">
-        <v>758</v>
+        <v>749</v>
       </c>
       <c r="AA81" t="s">
         <v>639</v>
       </c>
       <c r="AB81" t="s">
-        <v>871</v>
+        <v>862</v>
       </c>
       <c r="AC81" t="s">
-        <v>916</v>
+        <v>907</v>
       </c>
       <c r="AD81" t="s">
         <v>639</v>
       </c>
       <c r="AE81" t="s">
-        <v>936</v>
+        <v>927</v>
       </c>
     </row>
-    <row r="82" spans="1:49">
+    <row r="82" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -10955,20 +10873,17 @@
       <c r="X82" t="s">
         <v>689</v>
       </c>
-      <c r="Y82" t="s">
-        <v>701</v>
-      </c>
       <c r="Z82" t="s">
-        <v>759</v>
+        <v>750</v>
       </c>
       <c r="AA82" t="s">
         <v>639</v>
       </c>
       <c r="AB82" t="s">
-        <v>872</v>
+        <v>863</v>
       </c>
     </row>
-    <row r="83" spans="1:49">
+    <row r="83" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -11038,20 +10953,17 @@
       <c r="X83" t="s">
         <v>689</v>
       </c>
-      <c r="Y83" t="s">
-        <v>701</v>
-      </c>
       <c r="Z83" t="s">
-        <v>760</v>
+        <v>751</v>
       </c>
       <c r="AA83" t="s">
         <v>642</v>
       </c>
       <c r="AB83" t="s">
-        <v>873</v>
+        <v>864</v>
       </c>
     </row>
-    <row r="84" spans="1:49">
+    <row r="84" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -11121,20 +11033,17 @@
       <c r="X84" t="s">
         <v>689</v>
       </c>
-      <c r="Y84" t="s">
-        <v>701</v>
-      </c>
       <c r="Z84" t="s">
-        <v>761</v>
+        <v>752</v>
       </c>
       <c r="AA84" t="s">
         <v>639</v>
       </c>
       <c r="AB84" t="s">
-        <v>874</v>
+        <v>865</v>
       </c>
     </row>
-    <row r="85" spans="1:49">
+    <row r="85" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -11208,16 +11117,16 @@
         <v>687</v>
       </c>
       <c r="Z85" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
       <c r="AA85" t="s">
         <v>639</v>
       </c>
       <c r="AB85" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
-    <row r="86" spans="1:49">
+    <row r="86" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -11291,16 +11200,16 @@
         <v>687</v>
       </c>
       <c r="Z86" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="AA86" t="s">
         <v>639</v>
       </c>
       <c r="AB86" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
     </row>
-    <row r="87" spans="1:49">
+    <row r="87" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -11374,16 +11283,16 @@
         <v>687</v>
       </c>
       <c r="Z87" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="AA87" t="s">
         <v>639</v>
       </c>
       <c r="AB87" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
     </row>
-    <row r="88" spans="1:49">
+    <row r="88" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -11457,16 +11366,16 @@
         <v>687</v>
       </c>
       <c r="Z88" t="s">
-        <v>762</v>
+        <v>753</v>
       </c>
       <c r="AA88" t="s">
         <v>640</v>
       </c>
       <c r="AB88" t="s">
-        <v>875</v>
+        <v>866</v>
       </c>
     </row>
-    <row r="89" spans="1:49">
+    <row r="89" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -11536,14 +11445,11 @@
       <c r="X89" t="s">
         <v>689</v>
       </c>
-      <c r="Y89" t="s">
-        <v>701</v>
-      </c>
       <c r="Z89" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="AA89" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="AB89" t="s">
         <v>639</v>
@@ -11552,7 +11458,7 @@
         <v>640</v>
       </c>
       <c r="AD89" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
       <c r="AE89" t="s">
         <v>640</v>
@@ -11561,13 +11467,13 @@
         <v>640</v>
       </c>
       <c r="AV89" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
       <c r="AW89" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="90" spans="1:49">
+    <row r="90" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -11637,20 +11543,17 @@
       <c r="X90" t="s">
         <v>689</v>
       </c>
-      <c r="Y90" t="s">
-        <v>701</v>
-      </c>
       <c r="Z90" t="s">
-        <v>763</v>
+        <v>754</v>
       </c>
       <c r="AA90" t="s">
         <v>640</v>
       </c>
       <c r="AB90" t="s">
-        <v>876</v>
+        <v>867</v>
       </c>
     </row>
-    <row r="91" spans="1:49">
+    <row r="91" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -11720,29 +11623,26 @@
       <c r="X91" t="s">
         <v>689</v>
       </c>
-      <c r="Y91" t="s">
-        <v>701</v>
-      </c>
       <c r="Z91" t="s">
-        <v>764</v>
+        <v>755</v>
       </c>
       <c r="AA91" t="s">
         <v>639</v>
       </c>
       <c r="AB91" t="s">
-        <v>877</v>
+        <v>868</v>
       </c>
       <c r="AC91" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="AD91" t="s">
         <v>639</v>
       </c>
       <c r="AE91" t="s">
-        <v>937</v>
+        <v>928</v>
       </c>
     </row>
-    <row r="92" spans="1:49">
+    <row r="92" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -11812,20 +11712,17 @@
       <c r="X92" t="s">
         <v>689</v>
       </c>
-      <c r="Y92" t="s">
-        <v>701</v>
-      </c>
       <c r="Z92" t="s">
-        <v>765</v>
+        <v>756</v>
       </c>
       <c r="AA92" t="s">
         <v>640</v>
       </c>
       <c r="AB92" t="s">
-        <v>878</v>
+        <v>869</v>
       </c>
     </row>
-    <row r="93" spans="1:49">
+    <row r="93" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -11895,29 +11792,26 @@
       <c r="X93" t="s">
         <v>689</v>
       </c>
-      <c r="Y93" t="s">
-        <v>701</v>
-      </c>
       <c r="Z93" t="s">
-        <v>766</v>
+        <v>757</v>
       </c>
       <c r="AA93" t="s">
         <v>646</v>
       </c>
       <c r="AB93" t="s">
-        <v>879</v>
+        <v>870</v>
       </c>
       <c r="AC93" t="s">
-        <v>918</v>
+        <v>909</v>
       </c>
       <c r="AD93" t="s">
         <v>639</v>
       </c>
       <c r="AE93" t="s">
-        <v>938</v>
+        <v>929</v>
       </c>
     </row>
-    <row r="94" spans="1:49">
+    <row r="94" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -11987,29 +11881,26 @@
       <c r="X94" t="s">
         <v>689</v>
       </c>
-      <c r="Y94" t="s">
-        <v>701</v>
-      </c>
       <c r="Z94" t="s">
-        <v>767</v>
+        <v>758</v>
       </c>
       <c r="AA94" t="s">
         <v>640</v>
       </c>
       <c r="AB94" t="s">
-        <v>880</v>
+        <v>871</v>
       </c>
       <c r="AC94" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="AD94" t="s">
         <v>640</v>
       </c>
       <c r="AE94" t="s">
-        <v>939</v>
+        <v>930</v>
       </c>
     </row>
-    <row r="95" spans="1:49">
+    <row r="95" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -12079,20 +11970,17 @@
       <c r="X95" t="s">
         <v>689</v>
       </c>
-      <c r="Y95" t="s">
-        <v>701</v>
-      </c>
       <c r="Z95" t="s">
-        <v>768</v>
+        <v>759</v>
       </c>
       <c r="AA95" t="s">
         <v>639</v>
       </c>
       <c r="AB95" t="s">
-        <v>881</v>
+        <v>872</v>
       </c>
     </row>
-    <row r="96" spans="1:49">
+    <row r="96" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -12166,16 +12054,16 @@
         <v>692</v>
       </c>
       <c r="Z96" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
       <c r="AA96" t="s">
-        <v>816</v>
+        <v>807</v>
       </c>
       <c r="AB96" t="s">
-        <v>882</v>
+        <v>873</v>
       </c>
     </row>
-    <row r="97" spans="1:31">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -12249,16 +12137,16 @@
         <v>692</v>
       </c>
       <c r="Z97" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
       <c r="AA97" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="AB97" t="s">
-        <v>882</v>
+        <v>873</v>
       </c>
     </row>
-    <row r="98" spans="1:31">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -12332,16 +12220,16 @@
         <v>692</v>
       </c>
       <c r="Z98" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
       <c r="AA98" t="s">
-        <v>818</v>
+        <v>809</v>
       </c>
       <c r="AB98" t="s">
-        <v>882</v>
+        <v>873</v>
       </c>
     </row>
-    <row r="99" spans="1:31">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -12412,16 +12300,16 @@
         <v>692</v>
       </c>
       <c r="Z99" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
       <c r="AA99" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="AB99" t="s">
-        <v>883</v>
+        <v>874</v>
       </c>
     </row>
-    <row r="100" spans="1:31">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -12495,16 +12383,16 @@
         <v>692</v>
       </c>
       <c r="Z100" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
       <c r="AA100" t="s">
-        <v>819</v>
+        <v>810</v>
       </c>
       <c r="AB100" t="s">
-        <v>883</v>
+        <v>874</v>
       </c>
     </row>
-    <row r="101" spans="1:31">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -12578,16 +12466,16 @@
         <v>692</v>
       </c>
       <c r="Z101" t="s">
-        <v>770</v>
+        <v>761</v>
       </c>
       <c r="AA101" t="s">
-        <v>820</v>
+        <v>811</v>
       </c>
       <c r="AB101" t="s">
-        <v>884</v>
+        <v>875</v>
       </c>
     </row>
-    <row r="102" spans="1:31">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -12651,29 +12539,26 @@
       <c r="X102" t="s">
         <v>693</v>
       </c>
-      <c r="Y102" t="s">
-        <v>706</v>
-      </c>
       <c r="Z102" t="s">
-        <v>771</v>
+        <v>762</v>
       </c>
       <c r="AA102" t="s">
         <v>642</v>
       </c>
       <c r="AB102" t="s">
-        <v>885</v>
+        <v>876</v>
       </c>
       <c r="AC102" t="s">
-        <v>919</v>
+        <v>910</v>
       </c>
       <c r="AD102" t="s">
         <v>640</v>
       </c>
       <c r="AE102" t="s">
-        <v>940</v>
+        <v>931</v>
       </c>
     </row>
-    <row r="103" spans="1:31">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -12732,16 +12617,16 @@
         <v>693</v>
       </c>
       <c r="Z103" t="s">
-        <v>772</v>
+        <v>763</v>
       </c>
       <c r="AA103" t="s">
         <v>639</v>
       </c>
       <c r="AB103" t="s">
-        <v>886</v>
+        <v>877</v>
       </c>
     </row>
-    <row r="104" spans="1:31">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -12815,16 +12700,16 @@
         <v>693</v>
       </c>
       <c r="Z104" t="s">
-        <v>773</v>
+        <v>764</v>
       </c>
       <c r="AA104" t="s">
         <v>639</v>
       </c>
       <c r="AB104" t="s">
-        <v>887</v>
+        <v>878</v>
       </c>
     </row>
-    <row r="105" spans="1:31">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -12898,16 +12783,16 @@
         <v>693</v>
       </c>
       <c r="Z105" t="s">
-        <v>774</v>
+        <v>765</v>
       </c>
       <c r="AA105" t="s">
         <v>639</v>
       </c>
       <c r="AB105" t="s">
-        <v>888</v>
+        <v>879</v>
       </c>
     </row>
-    <row r="106" spans="1:31">
+    <row r="106" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -12981,16 +12866,16 @@
         <v>693</v>
       </c>
       <c r="Z106" t="s">
-        <v>775</v>
+        <v>766</v>
       </c>
       <c r="AA106" t="s">
         <v>639</v>
       </c>
       <c r="AB106" t="s">
-        <v>889</v>
+        <v>880</v>
       </c>
     </row>
-    <row r="107" spans="1:31">
+    <row r="107" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -13058,7 +12943,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="108" spans="1:31">
+    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -13126,7 +13011,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="109" spans="1:31">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -13200,16 +13085,16 @@
         <v>693</v>
       </c>
       <c r="Z109" t="s">
-        <v>776</v>
+        <v>767</v>
       </c>
       <c r="AA109" t="s">
         <v>640</v>
       </c>
       <c r="AB109" t="s">
-        <v>890</v>
+        <v>881</v>
       </c>
     </row>
-    <row r="110" spans="1:31">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -13280,16 +13165,16 @@
         <v>693</v>
       </c>
       <c r="Z110" t="s">
-        <v>777</v>
+        <v>768</v>
       </c>
       <c r="AA110" t="s">
-        <v>821</v>
+        <v>812</v>
       </c>
       <c r="AB110" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
     </row>
-    <row r="111" spans="1:31">
+    <row r="111" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -13360,16 +13245,16 @@
         <v>693</v>
       </c>
       <c r="Z111" t="s">
-        <v>777</v>
+        <v>768</v>
       </c>
       <c r="AA111" t="s">
-        <v>822</v>
+        <v>813</v>
       </c>
       <c r="AB111" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
     </row>
-    <row r="112" spans="1:31">
+    <row r="112" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -13434,25 +13319,25 @@
         <v>693</v>
       </c>
       <c r="Z112" t="s">
-        <v>778</v>
+        <v>769</v>
       </c>
       <c r="AA112" t="s">
         <v>639</v>
       </c>
       <c r="AB112" t="s">
-        <v>892</v>
+        <v>883</v>
       </c>
       <c r="AC112" t="s">
-        <v>920</v>
+        <v>911</v>
       </c>
       <c r="AD112" t="s">
         <v>639</v>
       </c>
       <c r="AE112" t="s">
-        <v>895</v>
+        <v>886</v>
       </c>
     </row>
-    <row r="113" spans="1:43">
+    <row r="113" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -13517,25 +13402,25 @@
         <v>693</v>
       </c>
       <c r="Z113" t="s">
-        <v>778</v>
+        <v>769</v>
       </c>
       <c r="AA113" t="s">
         <v>639</v>
       </c>
       <c r="AB113" t="s">
-        <v>892</v>
+        <v>883</v>
       </c>
       <c r="AC113" t="s">
-        <v>920</v>
+        <v>911</v>
       </c>
       <c r="AD113" t="s">
         <v>639</v>
       </c>
       <c r="AE113" t="s">
-        <v>895</v>
+        <v>886</v>
       </c>
     </row>
-    <row r="114" spans="1:43">
+    <row r="114" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -13606,7 +13491,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="115" spans="1:43">
+    <row r="115" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -13677,7 +13562,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="116" spans="1:43">
+    <row r="116" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -13748,16 +13633,16 @@
         <v>693</v>
       </c>
       <c r="Z116" t="s">
-        <v>779</v>
+        <v>770</v>
       </c>
       <c r="AA116" t="s">
         <v>639</v>
       </c>
       <c r="AB116" t="s">
-        <v>893</v>
+        <v>884</v>
       </c>
     </row>
-    <row r="117" spans="1:43">
+    <row r="117" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -13828,16 +13713,16 @@
         <v>693</v>
       </c>
       <c r="Z117" t="s">
-        <v>780</v>
+        <v>771</v>
       </c>
       <c r="AA117" t="s">
         <v>639</v>
       </c>
       <c r="AB117" t="s">
-        <v>894</v>
+        <v>885</v>
       </c>
     </row>
-    <row r="118" spans="1:43">
+    <row r="118" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -13908,16 +13793,16 @@
         <v>693</v>
       </c>
       <c r="Z118" t="s">
-        <v>781</v>
+        <v>772</v>
       </c>
       <c r="AA118" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
       <c r="AB118" t="s">
-        <v>895</v>
+        <v>886</v>
       </c>
     </row>
-    <row r="119" spans="1:43">
+    <row r="119" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -13991,16 +13876,16 @@
         <v>693</v>
       </c>
       <c r="Z119" t="s">
-        <v>782</v>
+        <v>773</v>
       </c>
       <c r="AA119" t="s">
         <v>639</v>
       </c>
       <c r="AB119" t="s">
-        <v>896</v>
+        <v>887</v>
       </c>
     </row>
-    <row r="120" spans="1:43">
+    <row r="120" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -14067,11 +13952,8 @@
       <c r="X120" t="s">
         <v>693</v>
       </c>
-      <c r="Y120" t="s">
-        <v>707</v>
-      </c>
     </row>
-    <row r="121" spans="1:43">
+    <row r="121" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -14145,16 +14027,16 @@
         <v>693</v>
       </c>
       <c r="Z121" t="s">
-        <v>783</v>
+        <v>774</v>
       </c>
       <c r="AA121" t="s">
         <v>639</v>
       </c>
       <c r="AB121" t="s">
-        <v>897</v>
+        <v>888</v>
       </c>
     </row>
-    <row r="122" spans="1:43">
+    <row r="122" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -14228,25 +14110,25 @@
         <v>693</v>
       </c>
       <c r="Z122" t="s">
-        <v>784</v>
+        <v>775</v>
       </c>
       <c r="AA122" t="s">
         <v>639</v>
       </c>
       <c r="AB122" t="s">
-        <v>898</v>
+        <v>889</v>
       </c>
       <c r="AC122" t="s">
-        <v>921</v>
+        <v>912</v>
       </c>
       <c r="AD122" t="s">
         <v>639</v>
       </c>
       <c r="AE122" t="s">
-        <v>941</v>
+        <v>932</v>
       </c>
     </row>
-    <row r="123" spans="1:43">
+    <row r="123" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -14316,20 +14198,17 @@
       <c r="X123" t="s">
         <v>694</v>
       </c>
-      <c r="Y123" t="s">
-        <v>708</v>
-      </c>
       <c r="Z123" t="s">
-        <v>785</v>
+        <v>776</v>
       </c>
       <c r="AA123" t="s">
         <v>639</v>
       </c>
       <c r="AB123" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
-    <row r="124" spans="1:43">
+    <row r="124" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -14396,38 +14275,35 @@
       <c r="X124" t="s">
         <v>694</v>
       </c>
-      <c r="Y124" t="s">
-        <v>708</v>
-      </c>
       <c r="Z124" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="AA124" t="s">
         <v>639</v>
       </c>
       <c r="AB124" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AC124" t="s">
-        <v>922</v>
+        <v>913</v>
       </c>
       <c r="AD124" t="s">
         <v>646</v>
       </c>
       <c r="AE124" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AF124" t="s">
-        <v>950</v>
+        <v>941</v>
       </c>
       <c r="AG124" t="s">
         <v>639</v>
       </c>
       <c r="AH124" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
     </row>
-    <row r="125" spans="1:43">
+    <row r="125" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -14497,47 +14373,44 @@
       <c r="X125" t="s">
         <v>694</v>
       </c>
-      <c r="Y125" t="s">
-        <v>708</v>
-      </c>
       <c r="Z125" t="s">
-        <v>787</v>
+        <v>778</v>
       </c>
       <c r="AA125" t="s">
         <v>639</v>
       </c>
       <c r="AB125" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AC125" t="s">
-        <v>922</v>
+        <v>913</v>
       </c>
       <c r="AD125" t="s">
         <v>646</v>
       </c>
       <c r="AE125" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AF125" t="s">
-        <v>950</v>
+        <v>941</v>
       </c>
       <c r="AG125" t="s">
         <v>639</v>
       </c>
       <c r="AH125" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AI125" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="AJ125" t="s">
         <v>639</v>
       </c>
       <c r="AK125" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
     </row>
-    <row r="126" spans="1:43">
+    <row r="126" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -14607,47 +14480,44 @@
       <c r="X126" t="s">
         <v>694</v>
       </c>
-      <c r="Y126" t="s">
-        <v>708</v>
-      </c>
       <c r="Z126" t="s">
-        <v>787</v>
+        <v>778</v>
       </c>
       <c r="AA126" t="s">
         <v>639</v>
       </c>
       <c r="AB126" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AC126" t="s">
-        <v>922</v>
+        <v>913</v>
       </c>
       <c r="AD126" t="s">
         <v>646</v>
       </c>
       <c r="AE126" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AF126" t="s">
-        <v>950</v>
+        <v>941</v>
       </c>
       <c r="AG126" t="s">
         <v>639</v>
       </c>
       <c r="AH126" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AI126" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="AJ126" t="s">
         <v>639</v>
       </c>
       <c r="AK126" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
     </row>
-    <row r="127" spans="1:43">
+    <row r="127" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -14717,47 +14587,44 @@
       <c r="X127" t="s">
         <v>694</v>
       </c>
-      <c r="Y127" t="s">
-        <v>708</v>
-      </c>
       <c r="Z127" t="s">
-        <v>787</v>
+        <v>778</v>
       </c>
       <c r="AA127" t="s">
         <v>639</v>
       </c>
       <c r="AB127" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AC127" t="s">
-        <v>922</v>
+        <v>913</v>
       </c>
       <c r="AD127" t="s">
         <v>646</v>
       </c>
       <c r="AE127" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AF127" t="s">
-        <v>950</v>
+        <v>941</v>
       </c>
       <c r="AG127" t="s">
         <v>639</v>
       </c>
       <c r="AH127" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="AI127" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="AJ127" t="s">
         <v>639</v>
       </c>
       <c r="AK127" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
     </row>
-    <row r="128" spans="1:43">
+    <row r="128" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -14827,65 +14694,62 @@
       <c r="X128" t="s">
         <v>694</v>
       </c>
-      <c r="Y128" t="s">
-        <v>708</v>
-      </c>
       <c r="Z128" t="s">
-        <v>788</v>
+        <v>779</v>
       </c>
       <c r="AA128" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
       <c r="AB128" t="s">
-        <v>901</v>
+        <v>892</v>
       </c>
       <c r="AC128" t="s">
-        <v>923</v>
+        <v>914</v>
       </c>
       <c r="AD128" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
       <c r="AE128" t="s">
+        <v>933</v>
+      </c>
+      <c r="AF128" t="s">
         <v>942</v>
       </c>
-      <c r="AF128" t="s">
-        <v>951</v>
-      </c>
       <c r="AG128" t="s">
         <v>639</v>
       </c>
       <c r="AH128" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
       <c r="AI128" t="s">
-        <v>969</v>
+        <v>960</v>
       </c>
       <c r="AJ128" t="s">
         <v>639</v>
       </c>
       <c r="AK128" t="s">
-        <v>974</v>
+        <v>965</v>
       </c>
       <c r="AL128" t="s">
-        <v>979</v>
+        <v>970</v>
       </c>
       <c r="AM128" t="s">
         <v>640</v>
       </c>
       <c r="AN128" t="s">
-        <v>986</v>
+        <v>977</v>
       </c>
       <c r="AO128" t="s">
-        <v>990</v>
+        <v>981</v>
       </c>
       <c r="AP128" t="s">
         <v>640</v>
       </c>
       <c r="AQ128" t="s">
-        <v>993</v>
+        <v>984</v>
       </c>
     </row>
-    <row r="129" spans="1:31">
+    <row r="129" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -14956,16 +14820,16 @@
         <v>695</v>
       </c>
       <c r="Z129" t="s">
-        <v>789</v>
+        <v>780</v>
       </c>
       <c r="AA129" t="s">
-        <v>824</v>
+        <v>815</v>
       </c>
       <c r="AB129" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
     </row>
-    <row r="130" spans="1:31">
+    <row r="130" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -15035,20 +14899,17 @@
       <c r="X130" t="s">
         <v>695</v>
       </c>
-      <c r="Y130" t="s">
-        <v>708</v>
-      </c>
       <c r="Z130" t="s">
-        <v>790</v>
+        <v>781</v>
       </c>
       <c r="AA130" t="s">
-        <v>825</v>
+        <v>816</v>
       </c>
       <c r="AB130" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
     </row>
-    <row r="131" spans="1:31">
+    <row r="131" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -15118,20 +14979,17 @@
       <c r="X131" t="s">
         <v>695</v>
       </c>
-      <c r="Y131" t="s">
-        <v>708</v>
-      </c>
       <c r="Z131" t="s">
-        <v>791</v>
+        <v>782</v>
       </c>
       <c r="AA131" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AB131" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
     </row>
-    <row r="132" spans="1:31">
+    <row r="132" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -15201,20 +15059,17 @@
       <c r="X132" t="s">
         <v>695</v>
       </c>
-      <c r="Y132" t="s">
-        <v>708</v>
-      </c>
       <c r="Z132" t="s">
-        <v>792</v>
+        <v>783</v>
       </c>
       <c r="AA132" t="s">
         <v>641</v>
       </c>
       <c r="AB132" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
     </row>
-    <row r="133" spans="1:31">
+    <row r="133" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -15284,20 +15139,17 @@
       <c r="X133" t="s">
         <v>695</v>
       </c>
-      <c r="Y133" t="s">
-        <v>708</v>
-      </c>
       <c r="Z133" t="s">
-        <v>793</v>
+        <v>784</v>
       </c>
       <c r="AA133" t="s">
-        <v>826</v>
+        <v>817</v>
       </c>
       <c r="AB133" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
     </row>
-    <row r="134" spans="1:31">
+    <row r="134" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -15371,13 +15223,13 @@
         <v>696</v>
       </c>
       <c r="Z134" t="s">
-        <v>794</v>
+        <v>785</v>
       </c>
       <c r="AB134" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
     </row>
-    <row r="135" spans="1:31">
+    <row r="135" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -15451,16 +15303,16 @@
         <v>697</v>
       </c>
       <c r="Z135" t="s">
-        <v>795</v>
+        <v>786</v>
       </c>
       <c r="AA135" t="s">
         <v>639</v>
       </c>
       <c r="AB135" t="s">
-        <v>888</v>
+        <v>879</v>
       </c>
     </row>
-    <row r="136" spans="1:31">
+    <row r="136" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -15533,29 +15385,26 @@
       <c r="X136" t="s">
         <v>697</v>
       </c>
-      <c r="Y136" t="s">
-        <v>709</v>
-      </c>
       <c r="Z136" t="s">
-        <v>796</v>
+        <v>787</v>
       </c>
       <c r="AA136" t="s">
         <v>646</v>
       </c>
       <c r="AB136" t="s">
-        <v>903</v>
+        <v>894</v>
       </c>
       <c r="AC136" t="s">
-        <v>924</v>
+        <v>915</v>
       </c>
       <c r="AD136" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AE136" t="s">
-        <v>903</v>
+        <v>894</v>
       </c>
     </row>
-    <row r="137" spans="1:31">
+    <row r="137" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -15629,25 +15478,25 @@
         <v>697</v>
       </c>
       <c r="Z137" t="s">
-        <v>796</v>
+        <v>787</v>
       </c>
       <c r="AA137" t="s">
         <v>646</v>
       </c>
       <c r="AB137" t="s">
-        <v>903</v>
+        <v>894</v>
       </c>
       <c r="AC137" t="s">
-        <v>924</v>
+        <v>915</v>
       </c>
       <c r="AD137" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="AE137" t="s">
-        <v>903</v>
+        <v>894</v>
       </c>
     </row>
-    <row r="138" spans="1:31">
+    <row r="138" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -15721,16 +15570,16 @@
         <v>697</v>
       </c>
       <c r="Z138" t="s">
-        <v>797</v>
+        <v>788</v>
       </c>
       <c r="AA138" t="s">
         <v>639</v>
       </c>
       <c r="AB138" t="s">
-        <v>904</v>
+        <v>895</v>
       </c>
     </row>
-    <row r="139" spans="1:31">
+    <row r="139" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -15803,20 +15652,17 @@
       <c r="X139" t="s">
         <v>698</v>
       </c>
-      <c r="Y139" t="s">
-        <v>702</v>
-      </c>
       <c r="Z139" t="s">
-        <v>798</v>
+        <v>789</v>
       </c>
       <c r="AA139" t="s">
         <v>639</v>
       </c>
       <c r="AB139" t="s">
-        <v>905</v>
+        <v>896</v>
       </c>
     </row>
-    <row r="140" spans="1:31">
+    <row r="140" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -15881,16 +15727,16 @@
         <v>696</v>
       </c>
       <c r="Z140" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
       <c r="AA140" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
       <c r="AB140" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
-    <row r="141" spans="1:31">
+    <row r="141" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -15955,13 +15801,13 @@
         <v>696</v>
       </c>
       <c r="Z141" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="AA141" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="AB141" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>